<commit_message>
Started working on unit tests.  Have about half of the entities complete. Fixed some bugs as a result of the testing.
</commit_message>
<xml_diff>
--- a/Endpoint definitions.xlsx
+++ b/Endpoint definitions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="222">
   <si>
     <t>Entity</t>
   </si>
@@ -684,6 +684,12 @@
   </si>
   <si>
     <t>"cards","_id","membersVoted"</t>
+  </si>
+  <si>
+    <t>BoardMembership</t>
+  </si>
+  <si>
+    <t>"boards","_boardId","memberships","_id"</t>
   </si>
 </sst>
 </file>
@@ -756,8 +762,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H153" totalsRowShown="0">
-  <autoFilter ref="A1:H153"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H155" totalsRowShown="0">
+  <autoFilter ref="A1:H155"/>
   <sortState ref="A2:H150">
     <sortCondition ref="A1:A150"/>
   </sortState>
@@ -1044,11 +1050,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H153"/>
+  <dimension ref="A1:H155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H71" sqref="H71"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H155" sqref="H155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5496,6 +5502,64 @@
         <v>{EntityRequestType.Token_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"tokens","_token"})},</v>
       </c>
     </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>220</v>
+      </c>
+      <c r="B154" t="s">
+        <v>11</v>
+      </c>
+      <c r="C154" t="s">
+        <v>4</v>
+      </c>
+      <c r="D154" s="1" t="str">
+        <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
+        <v>BoardMembership_Read_Refresh</v>
+      </c>
+      <c r="E154" s="1" t="str">
+        <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
+        <v>BoardMembership_Read_Refresh,</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H154" s="1" t="str">
+        <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
+        <v>{EntityRequestType.BoardMembership_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_boardId","memberships","_id"})},</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>5</v>
+      </c>
+      <c r="B155" t="s">
+        <v>11</v>
+      </c>
+      <c r="C155" t="s">
+        <v>4</v>
+      </c>
+      <c r="D155" s="1" t="str">
+        <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
+        <v>Attachment_Read_Refresh</v>
+      </c>
+      <c r="E155" s="1" t="str">
+        <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
+        <v>Attachment_Read_Refresh,</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H155" s="1" t="str">
+        <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
+        <v>{EntityRequestType.Attachment_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_cardId","attachments","_id"})},</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Completed rewrites of existing entity unit tests.
</commit_message>
<xml_diff>
--- a/Endpoint definitions.xlsx
+++ b/Endpoint definitions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="222">
   <si>
     <t>Entity</t>
   </si>
@@ -762,8 +762,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H155" totalsRowShown="0">
-  <autoFilter ref="A1:H155"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H156" totalsRowShown="0">
+  <autoFilter ref="A1:H156"/>
   <sortState ref="A2:H150">
     <sortCondition ref="A1:A150"/>
   </sortState>
@@ -1050,11 +1050,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H155"/>
+  <dimension ref="A1:H156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H155" sqref="H155"/>
+      <selection pane="bottomLeft" activeCell="F156" sqref="F156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5560,6 +5560,35 @@
         <v>{EntityRequestType.Attachment_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_cardId","attachments","_id"})},</v>
       </c>
     </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>66</v>
+      </c>
+      <c r="B156" t="s">
+        <v>12</v>
+      </c>
+      <c r="C156" t="s">
+        <v>8</v>
+      </c>
+      <c r="D156" s="1" t="str">
+        <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
+        <v>List_Write_Board</v>
+      </c>
+      <c r="E156" s="1" t="str">
+        <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
+        <v>List_Write_Board,</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G156" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H156" s="1" t="str">
+        <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
+        <v>{EntityRequestType.List_Write_Board, () =&gt; new Endpoint(RestMethod.Put, new[]{"lists","_id"})},</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished entity tests.  Started on internals testing. Still need solution to expose Action and Notification data.
</commit_message>
<xml_diff>
--- a/Endpoint definitions.xlsx
+++ b/Endpoint definitions.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Endpoints" sheetId="1" r:id="rId1"/>
+    <sheet name="Action Strings" sheetId="2" r:id="rId2"/>
+    <sheet name="Notification Strings" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="318">
   <si>
     <t>Entity</t>
   </si>
@@ -419,15 +421,6 @@
     <t>"checklists","_checkListId","checkItems","_id"</t>
   </si>
   <si>
-    <t>"cards","_cardId","checklists","_checkListId","checkItems","_id","name"</t>
-  </si>
-  <si>
-    <t>"cards","_cardId","checklists","_checkListId","checkItems","_id","pos"</t>
-  </si>
-  <si>
-    <t>"cards","_cardId","checklists","_checkListId","checkItems","_id","state"</t>
-  </si>
-  <si>
     <t>"checklists","_id","checkItems"</t>
   </si>
   <si>
@@ -690,6 +683,303 @@
   </si>
   <si>
     <t>"boards","_boardId","memberships","_id"</t>
+  </si>
+  <si>
+    <t>"cards","_cardId","checklist","_checkListId","checkItem","_id","name"</t>
+  </si>
+  <si>
+    <t>"cards","_cardId","checklist","_checkListId","checkItem","_id","pos"</t>
+  </si>
+  <si>
+    <t>"cards","_cardId","checklist","_checkListId","checkItem","_id","state"</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>AddAttachmentToCard</t>
+  </si>
+  <si>
+    <t>AddChecklistToCard</t>
+  </si>
+  <si>
+    <t>AddMemberToBoard</t>
+  </si>
+  <si>
+    <t>AddMemberToCard</t>
+  </si>
+  <si>
+    <t>AddMemberToOrganization</t>
+  </si>
+  <si>
+    <t>AddToOrganizationBoard</t>
+  </si>
+  <si>
+    <t>CommentCard</t>
+  </si>
+  <si>
+    <t>CopyCommentCard</t>
+  </si>
+  <si>
+    <t>ConvertToCardFromCheckItem</t>
+  </si>
+  <si>
+    <t>CopyBoard</t>
+  </si>
+  <si>
+    <t>CopyCard</t>
+  </si>
+  <si>
+    <t>CreateCard</t>
+  </si>
+  <si>
+    <t>CreateList</t>
+  </si>
+  <si>
+    <t>CreateOrganization</t>
+  </si>
+  <si>
+    <t>DeleteAttachmentFromCard</t>
+  </si>
+  <si>
+    <t>DeleteBoardInvitation</t>
+  </si>
+  <si>
+    <t>DeleteCard</t>
+  </si>
+  <si>
+    <t>DeleteOrganizationInvitation</t>
+  </si>
+  <si>
+    <t>MakeAdminOfBoard</t>
+  </si>
+  <si>
+    <t>MakeNormalMemberOfBoard</t>
+  </si>
+  <si>
+    <t>MakeNormalMemberOfOrganization</t>
+  </si>
+  <si>
+    <t>MakeObserverOfBoard</t>
+  </si>
+  <si>
+    <t>MemberJoinedTrello</t>
+  </si>
+  <si>
+    <t>MoveCardFromBoard</t>
+  </si>
+  <si>
+    <t>MoveListFromBoard</t>
+  </si>
+  <si>
+    <t>MoveCardToBoard</t>
+  </si>
+  <si>
+    <t>MoveListToBoard</t>
+  </si>
+  <si>
+    <t>RemoveAdminFromBoard</t>
+  </si>
+  <si>
+    <t>RemoveAdminFromOrganization</t>
+  </si>
+  <si>
+    <t>RemoveChecklistFromCard</t>
+  </si>
+  <si>
+    <t>RemoveFromOrganizationBoard</t>
+  </si>
+  <si>
+    <t>RemoveMemberFromBoard</t>
+  </si>
+  <si>
+    <t>RemoveMemberFromCard</t>
+  </si>
+  <si>
+    <t>UnconfirmedBoardInvitation</t>
+  </si>
+  <si>
+    <t>UnconfirmedOrganizationInvitation</t>
+  </si>
+  <si>
+    <t>UpdateBoard</t>
+  </si>
+  <si>
+    <t>UpdateCard</t>
+  </si>
+  <si>
+    <t>UpdateCheckItemStateOnCard</t>
+  </si>
+  <si>
+    <t>UpdateChecklist</t>
+  </si>
+  <si>
+    <t>UpdateMember</t>
+  </si>
+  <si>
+    <t>UpdateOrganization</t>
+  </si>
+  <si>
+    <t>UpdateCardIdList</t>
+  </si>
+  <si>
+    <t>UpdateCardClosed</t>
+  </si>
+  <si>
+    <t>UpdateCardDesc</t>
+  </si>
+  <si>
+    <t>UpdateCardName</t>
+  </si>
+  <si>
+    <t>{0} attached {1} to card {2}.</t>
+  </si>
+  <si>
+    <t>{0} added checklist {1} to card {2}.</t>
+  </si>
+  <si>
+    <t>{0} added member {1} to board {2}.</t>
+  </si>
+  <si>
+    <t>{0} assigned member {1} to card {2}.</t>
+  </si>
+  <si>
+    <t>{0} added member {1} to organization {2}.</t>
+  </si>
+  <si>
+    <t>{0} moved board {1} into organization {2}.</t>
+  </si>
+  <si>
+    <t>{0} commented on card {1}.</t>
+  </si>
+  <si>
+    <t>{0} converted checkitem {1} to a card.</t>
+  </si>
+  <si>
+    <t>{0} created board {1} from board {2}.</t>
+  </si>
+  <si>
+    <t>{0} created card {1} from card {2}.</t>
+  </si>
+  <si>
+    <t>{0} created board {1}.</t>
+  </si>
+  <si>
+    <t>{0} created card {1}.</t>
+  </si>
+  <si>
+    <t>{0} created list {1}.</t>
+  </si>
+  <si>
+    <t>{0} created organization {1}.</t>
+  </si>
+  <si>
+    <t>{0} removed attachment {1} from card {2}.</t>
+  </si>
+  <si>
+    <t>{0} rescinded an invitation to member {1} to join board {2}.</t>
+  </si>
+  <si>
+    <t>{0} deleted card {1}.</t>
+  </si>
+  <si>
+    <t>{0} rescinded an invitation to member {1} to join organization {2}.</t>
+  </si>
+  <si>
+    <t>{0} made member {1} an admin of board {2}.</t>
+  </si>
+  <si>
+    <t>{0} made member {1} a normal user of board {2}.</t>
+  </si>
+  <si>
+    <t>{0} made member {1} a normal user of organization {2}.</t>
+  </si>
+  <si>
+    <t>{0} made member {1} an observer of board {2}.</t>
+  </si>
+  <si>
+    <t>Three cheers for {0}: the newest member of Trello!</t>
+  </si>
+  <si>
+    <t>{0} moved card {1} from board {2} to board {3}.</t>
+  </si>
+  <si>
+    <t>{0} moved list {1} from board {2} to board {3}.</t>
+  </si>
+  <si>
+    <t>{0} removed member {1} as an admin of board {2}.</t>
+  </si>
+  <si>
+    <t>{0} removed member {1} as an admin of organization {2}.</t>
+  </si>
+  <si>
+    <t>{0} deleted checklist {1} from card {2}.</t>
+  </si>
+  <si>
+    <t>{0} removed board {1} from organization {0}.</t>
+  </si>
+  <si>
+    <t>{0} removed member {1} from board {2}.</t>
+  </si>
+  <si>
+    <t>{0} removed member {1} from card {2}.</t>
+  </si>
+  <si>
+    <t>{0} invited Trello outsider {1} to join the board.</t>
+  </si>
+  <si>
+    <t>{0} invited Trello outsider {1} to join the organization.</t>
+  </si>
+  <si>
+    <t>{0} updated board {1}.</t>
+  </si>
+  <si>
+    <t>{0} updated card {1}.</t>
+  </si>
+  <si>
+    <t>{0} updated checkitem {1}.</t>
+  </si>
+  <si>
+    <t>{0} updated checklist {1}.</t>
+  </si>
+  <si>
+    <t>{0} updated organization {1}.</t>
+  </si>
+  <si>
+    <t>{0} updated their profile.</t>
+  </si>
+  <si>
+    <t>{0} moved card {1} to list {2}.</t>
+  </si>
+  <si>
+    <t>{0} archived card {1}.</t>
+  </si>
+  <si>
+    <t>{0} changed the description of card {1}.</t>
+  </si>
+  <si>
+    <t>{0} changed the name of card {1} to {2}.</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>"card.idShort"</t>
+  </si>
+  <si>
+    <t>"checklist.name","card.name"</t>
+  </si>
+  <si>
+    <t>"organization.name"</t>
+  </si>
+  <si>
+    <t>"board.name"</t>
+  </si>
+  <si>
+    <t>"board.name","organization.name"</t>
   </si>
 </sst>
 </file>
@@ -1052,9 +1342,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F156" sqref="F156"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,7 +1378,7 @@
         <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H1" t="s">
         <v>34</v>
@@ -1145,7 +1435,7 @@
         <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H3" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1203,7 +1493,7 @@
         <v>103</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H5" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1218,21 +1508,21 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
+        <v>Board_Read_Actions</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
+        <v>Board_Read_Actions,</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D6" s="1" t="str">
-        <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Read_Actions</v>
-      </c>
-      <c r="E6" s="1" t="str">
-        <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Read_Actions,</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H6" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1261,7 +1551,7 @@
         <v>104</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H7" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1290,7 +1580,7 @@
         <v>105</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H8" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1305,7 +1595,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D9" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -1316,10 +1606,10 @@
         <v>Board_Read_Cards,</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H9" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1334,7 +1624,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D10" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -1345,10 +1635,10 @@
         <v>Board_Read_Checklists,</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H10" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1377,7 +1667,7 @@
         <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H11" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1392,7 +1682,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D12" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -1403,10 +1693,10 @@
         <v>Board_Read_InvitedMembers,</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H12" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1435,7 +1725,7 @@
         <v>108</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H13" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1464,7 +1754,7 @@
         <v>33</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H14" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1493,7 +1783,7 @@
         <v>33</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H15" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1522,7 +1812,7 @@
         <v>33</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H16" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1537,7 +1827,7 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D17" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -1548,10 +1838,10 @@
         <v>Board_Read_Lists,</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H17" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1580,7 +1870,7 @@
         <v>106</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H18" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1595,7 +1885,7 @@
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D19" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -1609,7 +1899,7 @@
         <v>105</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H19" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1624,7 +1914,7 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D20" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -1635,10 +1925,10 @@
         <v>Board_Read_Memberships,</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H20" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1667,7 +1957,7 @@
         <v>33</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H21" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1696,7 +1986,7 @@
         <v>33</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H22" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1725,7 +2015,7 @@
         <v>33</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H23" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1812,7 +2102,7 @@
         <v>109</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H26" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1841,7 +2131,7 @@
         <v>110</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H27" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1870,7 +2160,7 @@
         <v>111</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H28" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1899,7 +2189,7 @@
         <v>112</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H29" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1928,7 +2218,7 @@
         <v>113</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H30" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1957,7 +2247,7 @@
         <v>114</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H31" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -1986,7 +2276,7 @@
         <v>115</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H32" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2015,7 +2305,7 @@
         <v>117</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H33" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2044,7 +2334,7 @@
         <v>118</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H34" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2073,7 +2363,7 @@
         <v>119</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H35" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2102,7 +2392,7 @@
         <v>120</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H36" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2131,7 +2421,7 @@
         <v>116</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H37" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2160,7 +2450,7 @@
         <v>121</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H38" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2175,7 +2465,7 @@
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D39" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -2186,10 +2476,10 @@
         <v>Card_Read_Actions,</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H39" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2218,7 +2508,7 @@
         <v>122</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H40" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2244,10 +2534,10 @@
         <v>Card_Write_AddChecklist,</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H41" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2276,7 +2566,7 @@
         <v>124</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H42" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2305,7 +2595,7 @@
         <v>125</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H43" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2334,7 +2624,7 @@
         <v>126</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H44" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2349,7 +2639,7 @@
         <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D45" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -2363,7 +2653,7 @@
         <v>122</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H45" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2378,7 +2668,7 @@
         <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D46" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -2389,10 +2679,10 @@
         <v>Card_Read_CheckItems,</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H46" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2407,7 +2697,7 @@
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D47" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -2418,10 +2708,10 @@
         <v>Card_Read_Checklists,</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H47" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2450,7 +2740,7 @@
         <v>127</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H48" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2508,7 +2798,7 @@
         <v>123</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H50" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2537,7 +2827,7 @@
         <v>123</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H51" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2566,7 +2856,7 @@
         <v>123</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H52" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2595,7 +2885,7 @@
         <v>123</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H53" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2610,7 +2900,7 @@
         <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D54" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -2624,7 +2914,7 @@
         <v>125</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H54" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2639,7 +2929,7 @@
         <v>11</v>
       </c>
       <c r="C55" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D55" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -2650,10 +2940,10 @@
         <v>Card_Read_Members,</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H55" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2682,7 +2972,7 @@
         <v>123</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H56" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2711,7 +3001,7 @@
         <v>123</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H57" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2740,7 +3030,7 @@
         <v>123</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H58" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2769,7 +3059,7 @@
         <v>123</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H59" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2842,7 +3132,7 @@
         <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D62" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -2853,10 +3143,10 @@
         <v>Card_Read_VotingMembers,</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H62" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2885,7 +3175,7 @@
         <v>123</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H63" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -2940,14 +3230,14 @@
         <v>CheckItem_Write_Name,</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>131</v>
+        <v>219</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H65" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.CheckItem_Write_Name, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_cardId","checklists","_checkListId","checkItems","_id","name"})},</v>
+        <v>{EntityRequestType.CheckItem_Write_Name, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_cardId","checklist","_checkListId","checkItem","_id","name"})},</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2969,14 +3259,14 @@
         <v>CheckItem_Write_Position,</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>132</v>
+        <v>220</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H66" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.CheckItem_Write_Position, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_cardId","checklists","_checkListId","checkItems","_id","pos"})},</v>
+        <v>{EntityRequestType.CheckItem_Write_Position, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_cardId","checklist","_checkListId","checkItem","_id","pos"})},</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -3001,7 +3291,7 @@
         <v>130</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H67" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3027,14 +3317,14 @@
         <v>CheckItem_Write_State,</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>133</v>
+        <v>221</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H68" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.CheckItem_Write_State, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_cardId","checklists","_checkListId","checkItems","_id","state"})},</v>
+        <v>{EntityRequestType.CheckItem_Write_State, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_cardId","checklist","_checkListId","checkItem","_id","state"})},</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -3056,10 +3346,10 @@
         <v>CheckList_Write_AddCheckItem,</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H69" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3085,10 +3375,10 @@
         <v>CheckList_Write_Card,</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H70" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3103,7 +3393,7 @@
         <v>11</v>
       </c>
       <c r="C71" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D71" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -3114,10 +3404,10 @@
         <v>CheckList_Read_CheckItems,</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H71" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3143,7 +3433,7 @@
         <v>CheckList_Write_Delete,</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>17</v>
@@ -3172,10 +3462,10 @@
         <v>CheckList_Write_Name,</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H73" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3201,10 +3491,10 @@
         <v>CheckList_Write_Position,</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H74" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3230,10 +3520,10 @@
         <v>CheckList_Read_Refresh,</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H75" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3262,7 +3552,7 @@
         <v>108</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H76" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3271,7 +3561,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B77" t="s">
         <v>12</v>
@@ -3288,10 +3578,10 @@
         <v>LabelNames_Write_Blue,</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H77" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3300,7 +3590,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B78" t="s">
         <v>12</v>
@@ -3317,10 +3607,10 @@
         <v>LabelNames_Write_Green,</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H78" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3329,7 +3619,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B79" t="s">
         <v>12</v>
@@ -3346,10 +3636,10 @@
         <v>LabelNames_Write_Orange,</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H79" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3358,7 +3648,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B80" t="s">
         <v>12</v>
@@ -3375,10 +3665,10 @@
         <v>LabelNames_Write_Purple,</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H80" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3387,7 +3677,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B81" t="s">
         <v>12</v>
@@ -3404,10 +3694,10 @@
         <v>LabelNames_Write_Red,</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H81" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3416,7 +3706,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B82" t="s">
         <v>11</v>
@@ -3433,10 +3723,10 @@
         <v>LabelNames_Read_Refresh,</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H82" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3445,7 +3735,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B83" t="s">
         <v>12</v>
@@ -3462,10 +3752,10 @@
         <v>LabelNames_Write_Yellow,</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H83" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3480,7 +3770,7 @@
         <v>11</v>
       </c>
       <c r="C84" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D84" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -3491,10 +3781,10 @@
         <v>List_Read_Actions,</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H84" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3520,10 +3810,10 @@
         <v>List_Write_AddCard,</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H85" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3538,7 +3828,7 @@
         <v>11</v>
       </c>
       <c r="C86" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D86" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -3549,10 +3839,10 @@
         <v>List_Read_Cards,</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H86" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3578,7 +3868,7 @@
         <v>List_Write_Delete,</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>17</v>
@@ -3607,10 +3897,10 @@
         <v>List_Write_IsClosed,</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H88" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3636,10 +3926,10 @@
         <v>List_Write_IsSubscribed,</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H89" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3665,10 +3955,10 @@
         <v>List_Write_Move,</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H90" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3694,10 +3984,10 @@
         <v>List_Write_Name,</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H91" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3723,10 +4013,10 @@
         <v>List_Write_Position,</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H92" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3752,10 +4042,10 @@
         <v>List_Read_Refresh,</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H93" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3770,7 +4060,7 @@
         <v>11</v>
       </c>
       <c r="C94" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D94" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -3781,10 +4071,10 @@
         <v>Member_Read_Actions,</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H94" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3810,10 +4100,10 @@
         <v>Member_Write_AvatarSource,</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H95" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3839,10 +4129,10 @@
         <v>Member_Write_Bio,</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H96" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3857,7 +4147,7 @@
         <v>11</v>
       </c>
       <c r="C97" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D97" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -3868,10 +4158,10 @@
         <v>Member_Read_Boards,</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H97" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3886,7 +4176,7 @@
         <v>11</v>
       </c>
       <c r="C98" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D98" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -3897,10 +4187,10 @@
         <v>Member_Read_Cards,</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H98" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3926,10 +4216,10 @@
         <v>Member_Write_ClearNotifications,</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H99" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3955,10 +4245,10 @@
         <v>Member_Write_CreateBoard,</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H100" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -3984,10 +4274,10 @@
         <v>Member_Write_CreateOrganizations,</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H101" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4013,10 +4303,10 @@
         <v>Member_Write_FullName,</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H102" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4042,10 +4332,10 @@
         <v>Member_Write_Initials,</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H103" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4060,7 +4350,7 @@
         <v>11</v>
       </c>
       <c r="C104" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D104" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -4071,10 +4361,10 @@
         <v>Member_Read_InvitedBoards,</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H104" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4089,7 +4379,7 @@
         <v>11</v>
       </c>
       <c r="C105" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D105" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -4100,10 +4390,10 @@
         <v>Member_Read_InvitedOrganizations,</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H105" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4118,7 +4408,7 @@
         <v>11</v>
       </c>
       <c r="C106" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D106" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -4129,10 +4419,10 @@
         <v>Member_Read_Notifications,</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H106" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4158,10 +4448,10 @@
         <v>Member_Read_Organization,</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H107" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4187,10 +4477,10 @@
         <v>Member_Write_PinBoard,</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H108" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4216,10 +4506,10 @@
         <v>Member_Read_Refresh,</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H109" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4245,7 +4535,7 @@
         <v>Member_Write_RescindVoteForCard,</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G110" s="1" t="s">
         <v>17</v>
@@ -4263,7 +4553,7 @@
         <v>11</v>
       </c>
       <c r="C111" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D111" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -4274,10 +4564,10 @@
         <v>Member_Read_Sessions,</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H111" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4292,7 +4582,7 @@
         <v>11</v>
       </c>
       <c r="C112" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D112" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -4303,10 +4593,10 @@
         <v>Member_Read_Tokens,</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H112" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4332,7 +4622,7 @@
         <v>Member_Write_UnpinBoard,</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>17</v>
@@ -4361,10 +4651,10 @@
         <v>Member_Write_Username,</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H114" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4390,10 +4680,10 @@
         <v>Member_Write_VoteForCard,</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H115" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4419,10 +4709,10 @@
         <v>MemberPreferences_Write_ColorBlind,</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H116" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4448,10 +4738,10 @@
         <v>MemberPreferences_Write_MinutesBeforeDeadlineToNotify,</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H117" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4477,10 +4767,10 @@
         <v>MemberPreferences_Write_MinutesBetweenSummaries,</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H118" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4506,10 +4796,10 @@
         <v>MemberPreferences_Read_Refresh,</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H119" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4535,10 +4825,10 @@
         <v>MemberPreferences_Write_SendSummaries,</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H120" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4564,7 +4854,7 @@
         <v>MemberSession_Write_Delete,</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G121" s="1" t="s">
         <v>17</v>
@@ -4593,10 +4883,10 @@
         <v>Notification_Write_IsUnread,</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H122" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4622,10 +4912,10 @@
         <v>Notification_Read_Refresh,</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H123" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4640,7 +4930,7 @@
         <v>11</v>
       </c>
       <c r="C124" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D124" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -4651,10 +4941,10 @@
         <v>Organization_Read_Actions,</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H124" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4680,10 +4970,10 @@
         <v>Organization_Write_AddOrUpdateMember,</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H125" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4698,7 +4988,7 @@
         <v>11</v>
       </c>
       <c r="C126" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D126" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -4709,10 +4999,10 @@
         <v>Organization_Read_Boards,</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H126" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4738,10 +5028,10 @@
         <v>Organization_Write_CreateBoard,</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H127" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4767,7 +5057,7 @@
         <v>Organization_Write_Delete,</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>17</v>
@@ -4796,10 +5086,10 @@
         <v>Organization_Write_Description,</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H129" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4825,10 +5115,10 @@
         <v>Organization_Write_DisplayName,</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H130" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4843,7 +5133,7 @@
         <v>11</v>
       </c>
       <c r="C131" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D131" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -4854,10 +5144,10 @@
         <v>Organization_Read_InvitedMembers,</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H131" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4886,7 +5176,7 @@
         <v>108</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H132" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4901,7 +5191,7 @@
         <v>11</v>
       </c>
       <c r="C133" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D133" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -4912,10 +5202,10 @@
         <v>Organization_Read_Members,</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H133" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4930,7 +5220,7 @@
         <v>11</v>
       </c>
       <c r="C134" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D134" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
@@ -4941,10 +5231,10 @@
         <v>Organization_Read_Memberships,</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H134" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4970,10 +5260,10 @@
         <v>Organization_Write_Name,</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H135" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -4999,10 +5289,10 @@
         <v>Organization_Read_Refresh,</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H136" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5028,7 +5318,7 @@
         <v>Organization_Write_RemoveMember,</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G137" s="1" t="s">
         <v>17</v>
@@ -5086,10 +5376,10 @@
         <v>Organization_Write_Website,</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H139" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5115,10 +5405,10 @@
         <v>OrganizationMembership_Read_Refresh,</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H140" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5144,10 +5434,10 @@
         <v>OrganizationPreferences_Write_AssociatedDomain,</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H141" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5173,10 +5463,10 @@
         <v>OrganizationPreferences_Write_ExternalMembersDisabled,</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H142" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5202,10 +5492,10 @@
         <v>OrganizationPreferences_Write_OrgInviteRestrict,</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H143" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5231,10 +5521,10 @@
         <v>OrganizationPreferences_Write_OrgVisibleBoardVisibility,</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H144" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5260,10 +5550,10 @@
         <v>OrganizationPreferences_Write_PermissionLevel,</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H145" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5289,10 +5579,10 @@
         <v>OrganizationPreferences_Write_PrivateBoardVisibility,</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H146" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5318,10 +5608,10 @@
         <v>OrganizationPreferences_Write_PublicBoardVisibility,</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H147" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5347,10 +5637,10 @@
         <v>OrganizationPreferences_Read_Refresh,</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H148" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5376,10 +5666,10 @@
         <v>Service_Read_Me,</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H149" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5405,10 +5695,10 @@
         <v>Service_Read_Search,</v>
       </c>
       <c r="F150" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G150" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="G150" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="H150" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5434,10 +5724,10 @@
         <v>Service_Read_SearchMembers,</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H151" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5463,7 +5753,7 @@
         <v>Token_Write_Delete,</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G152" s="1" t="s">
         <v>17</v>
@@ -5492,10 +5782,10 @@
         <v>Token_Read_Refresh,</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H153" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5504,7 +5794,7 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B154" t="s">
         <v>11</v>
@@ -5521,10 +5811,10 @@
         <v>BoardMembership_Read_Refresh,</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H154" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5553,7 +5843,7 @@
         <v>102</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H155" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5579,10 +5869,10 @@
         <v>List_Write_Board,</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H156" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
@@ -5596,4 +5886,616 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.42578125" customWidth="1"/>
+    <col min="4" max="4" width="86.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"{ActionType."&amp;A2&amp;", a =&gt; BuildString(a, """&amp;B2&amp;""", "&amp;C2&amp;")},"</f>
+        <v>{ActionType.AddAttachmentToCard, a =&gt; BuildString(a, "{0} attached {1} to card {2}.", )},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" t="s">
+        <v>270</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D47" si="0">"{ActionType."&amp;A3&amp;", a =&gt; BuildString(a, """&amp;B3&amp;""", "&amp;C3&amp;")},"</f>
+        <v>{ActionType.AddChecklistToCard, a =&gt; BuildString(a, "{0} added checklist {1} to card {2}.", )},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.AddMemberToBoard, a =&gt; BuildString(a, "{0} added member {1} to board {2}.", )},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.AddMemberToCard, a =&gt; BuildString(a, "{0} assigned member {1} to card {2}.", )},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" t="s">
+        <v>273</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.AddMemberToOrganization, a =&gt; BuildString(a, "{0} added member {1} to organization {2}.", )},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" t="s">
+        <v>317</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.AddToOrganizationBoard, a =&gt; BuildString(a, "{0} moved board {1} into organization {2}.", "board.name","organization.name")},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.CommentCard, a =&gt; BuildString(a, "{0} commented on card {1}.", )},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.CopyCommentCard, a =&gt; BuildString(a, "", )},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" t="s">
+        <v>276</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.ConvertToCardFromCheckItem, a =&gt; BuildString(a, "{0} converted checkitem {1} to a card.", )},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B11" t="s">
+        <v>277</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.CopyBoard, a =&gt; BuildString(a, "{0} created board {1} from board {2}.", )},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>234</v>
+      </c>
+      <c r="B12" t="s">
+        <v>278</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.CopyCard, a =&gt; BuildString(a, "{0} created card {1} from card {2}.", )},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
+        <v>279</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.CreateBoard, a =&gt; BuildString(a, "{0} created board {1}.", )},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>235</v>
+      </c>
+      <c r="B14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.CreateCard, a =&gt; BuildString(a, "{0} created card {1}.", )},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>236</v>
+      </c>
+      <c r="B15" t="s">
+        <v>281</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.CreateList, a =&gt; BuildString(a, "{0} created list {1}.", )},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>237</v>
+      </c>
+      <c r="B16" t="s">
+        <v>282</v>
+      </c>
+      <c r="C16" t="s">
+        <v>315</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.CreateOrganization, a =&gt; BuildString(a, "{0} created organization {1}.", "organization.name")},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>238</v>
+      </c>
+      <c r="B17" t="s">
+        <v>283</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.DeleteAttachmentFromCard, a =&gt; BuildString(a, "{0} removed attachment {1} from card {2}.", )},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>239</v>
+      </c>
+      <c r="B18" t="s">
+        <v>284</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.DeleteBoardInvitation, a =&gt; BuildString(a, "{0} rescinded an invitation to member {1} to join board {2}.", )},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>240</v>
+      </c>
+      <c r="B19" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" t="s">
+        <v>313</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.DeleteCard, a =&gt; BuildString(a, "{0} deleted card {1}.", "card.idShort")},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>241</v>
+      </c>
+      <c r="B20" t="s">
+        <v>286</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.DeleteOrganizationInvitation, a =&gt; BuildString(a, "{0} rescinded an invitation to member {1} to join organization {2}.", )},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>242</v>
+      </c>
+      <c r="B21" t="s">
+        <v>287</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.MakeAdminOfBoard, a =&gt; BuildString(a, "{0} made member {1} an admin of board {2}.", )},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>243</v>
+      </c>
+      <c r="B22" t="s">
+        <v>288</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.MakeNormalMemberOfBoard, a =&gt; BuildString(a, "{0} made member {1} a normal user of board {2}.", )},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>244</v>
+      </c>
+      <c r="B23" t="s">
+        <v>289</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.MakeNormalMemberOfOrganization, a =&gt; BuildString(a, "{0} made member {1} a normal user of organization {2}.", )},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>245</v>
+      </c>
+      <c r="B24" t="s">
+        <v>290</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.MakeObserverOfBoard, a =&gt; BuildString(a, "{0} made member {1} an observer of board {2}.", )},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>246</v>
+      </c>
+      <c r="B25" t="s">
+        <v>291</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.MemberJoinedTrello, a =&gt; BuildString(a, "Three cheers for {0}: the newest member of Trello!", )},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>247</v>
+      </c>
+      <c r="B26" t="s">
+        <v>292</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.MoveCardFromBoard, a =&gt; BuildString(a, "{0} moved card {1} from board {2} to board {3}.", )},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>248</v>
+      </c>
+      <c r="B27" t="s">
+        <v>293</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.MoveListFromBoard, a =&gt; BuildString(a, "{0} moved list {1} from board {2} to board {3}.", )},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>249</v>
+      </c>
+      <c r="B28" t="s">
+        <v>292</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.MoveCardToBoard, a =&gt; BuildString(a, "{0} moved card {1} from board {2} to board {3}.", )},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>250</v>
+      </c>
+      <c r="B29" t="s">
+        <v>293</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.MoveListToBoard, a =&gt; BuildString(a, "{0} moved list {1} from board {2} to board {3}.", )},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>251</v>
+      </c>
+      <c r="B30" t="s">
+        <v>294</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.RemoveAdminFromBoard, a =&gt; BuildString(a, "{0} removed member {1} as an admin of board {2}.", )},</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>252</v>
+      </c>
+      <c r="B31" t="s">
+        <v>295</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.RemoveAdminFromOrganization, a =&gt; BuildString(a, "{0} removed member {1} as an admin of organization {2}.", )},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>253</v>
+      </c>
+      <c r="B32" t="s">
+        <v>296</v>
+      </c>
+      <c r="C32" t="s">
+        <v>314</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.RemoveChecklistFromCard, a =&gt; BuildString(a, "{0} deleted checklist {1} from card {2}.", "checklist.name","card.name")},</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>254</v>
+      </c>
+      <c r="B33" t="s">
+        <v>297</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.RemoveFromOrganizationBoard, a =&gt; BuildString(a, "{0} removed board {1} from organization {0}.", )},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>255</v>
+      </c>
+      <c r="B34" t="s">
+        <v>298</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.RemoveMemberFromBoard, a =&gt; BuildString(a, "{0} removed member {1} from board {2}.", )},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>256</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.RemoveMemberFromCard, a =&gt; BuildString(a, "{0} removed member {1} from card {2}.", )},</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>257</v>
+      </c>
+      <c r="B36" t="s">
+        <v>300</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.UnconfirmedBoardInvitation, a =&gt; BuildString(a, "{0} invited Trello outsider {1} to join the board.", )},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>258</v>
+      </c>
+      <c r="B37" t="s">
+        <v>301</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.UnconfirmedOrganizationInvitation, a =&gt; BuildString(a, "{0} invited Trello outsider {1} to join the organization.", )},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>259</v>
+      </c>
+      <c r="B38" t="s">
+        <v>302</v>
+      </c>
+      <c r="C38" t="s">
+        <v>316</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.UpdateBoard, a =&gt; BuildString(a, "{0} updated board {1}.", "board.name")},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>260</v>
+      </c>
+      <c r="B39" t="s">
+        <v>303</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.UpdateCard, a =&gt; BuildString(a, "{0} updated card {1}.", )},</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>261</v>
+      </c>
+      <c r="B40" t="s">
+        <v>304</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.UpdateCheckItemStateOnCard, a =&gt; BuildString(a, "{0} updated checkitem {1}.", )},</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>262</v>
+      </c>
+      <c r="B41" t="s">
+        <v>305</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.UpdateChecklist, a =&gt; BuildString(a, "{0} updated checklist {1}.", )},</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>263</v>
+      </c>
+      <c r="B42" t="s">
+        <v>307</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.UpdateMember, a =&gt; BuildString(a, "{0} updated their profile.", )},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>264</v>
+      </c>
+      <c r="B43" t="s">
+        <v>306</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.UpdateOrganization, a =&gt; BuildString(a, "{0} updated organization {1}.", )},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>265</v>
+      </c>
+      <c r="B44" t="s">
+        <v>308</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.UpdateCardIdList, a =&gt; BuildString(a, "{0} moved card {1} to list {2}.", )},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>266</v>
+      </c>
+      <c r="B45" t="s">
+        <v>309</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.UpdateCardClosed, a =&gt; BuildString(a, "{0} archived card {1}.", )},</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>267</v>
+      </c>
+      <c r="B46" t="s">
+        <v>310</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.UpdateCardDesc, a =&gt; BuildString(a, "{0} changed the description of card {1}.", )},</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>268</v>
+      </c>
+      <c r="B47" t="s">
+        <v>311</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>{ActionType.UpdateCardName, a =&gt; BuildString(a, "{0} changed the name of card {1} to {2}.", )},</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed implementation of Action and Notification. BUG FIX: Requesting an entity that doesn't exist causes crash or hang
</commit_message>
<xml_diff>
--- a/Endpoint definitions.xlsx
+++ b/Endpoint definitions.xlsx
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Action Strings'!$A$1:$D$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Notification Strings'!$A$1:$D$25</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="376">
   <si>
     <t>Entity</t>
   </si>
@@ -856,18 +857,9 @@
     <t>{0} moved board {1} into organization {2}.</t>
   </si>
   <si>
-    <t>{0} commented on card {1}.</t>
-  </si>
-  <si>
     <t>{0} converted checkitem {1} to a card.</t>
   </si>
   <si>
-    <t>{0} created board {1} from board {2}.</t>
-  </si>
-  <si>
-    <t>{0} created card {1} from card {2}.</t>
-  </si>
-  <si>
     <t>{0} created board {1}.</t>
   </si>
   <si>
@@ -970,55 +962,202 @@
     <t>{0} moved card {1} from list {2} to list {3}.</t>
   </si>
   <si>
-    <t>a.Attachment, a.Card</t>
-  </si>
-  <si>
-    <t>a.CheckList, a.Card</t>
-  </si>
-  <si>
-    <t>a.Member, a.Board</t>
-  </si>
-  <si>
-    <t>a.Member, a.Card</t>
-  </si>
-  <si>
-    <t>a.Member, a.Organization</t>
-  </si>
-  <si>
-    <t>a.Board, a.Organization</t>
-  </si>
-  <si>
-    <t>a.Card</t>
-  </si>
-  <si>
-    <t>a.CheckItem</t>
-  </si>
-  <si>
-    <t>a.Board, a.SourceBoard</t>
-  </si>
-  <si>
-    <t>a.Card, a.SourceCard</t>
-  </si>
-  <si>
-    <t>a.Board</t>
-  </si>
-  <si>
-    <t>a.List</t>
-  </si>
-  <si>
-    <t>a.Organization</t>
-  </si>
-  <si>
-    <t>a.CardShortId, a.Board</t>
-  </si>
-  <si>
-    <t>a.CheckList</t>
-  </si>
-  <si>
-    <t>a.Card, a.ListBefore, a.ListAfter</t>
-  </si>
-  <si>
     <t>{0} removed board {1} from organization {2}.</t>
+  </si>
+  <si>
+    <t>{0} copied card {1} from card {2}.</t>
+  </si>
+  <si>
+    <t>{0} copied board {1} from board {2}.</t>
+  </si>
+  <si>
+    <t>AddedAttachmentToCard</t>
+  </si>
+  <si>
+    <t>AddedToBoard</t>
+  </si>
+  <si>
+    <t>AddedToCard</t>
+  </si>
+  <si>
+    <t>AddedToOrganization</t>
+  </si>
+  <si>
+    <t>AddedMemberToCard</t>
+  </si>
+  <si>
+    <t>AddAdminToBoard</t>
+  </si>
+  <si>
+    <t>AddAdminToOrganization</t>
+  </si>
+  <si>
+    <t>ChangeCard</t>
+  </si>
+  <si>
+    <t>CloseBoard</t>
+  </si>
+  <si>
+    <t>CreatedCard</t>
+  </si>
+  <si>
+    <t>InvitedToBoard</t>
+  </si>
+  <si>
+    <t>InvitedToOrganization</t>
+  </si>
+  <si>
+    <t>RemovedFromBoard</t>
+  </si>
+  <si>
+    <t>RemovedFromCard</t>
+  </si>
+  <si>
+    <t>RemovedMemberFromCard</t>
+  </si>
+  <si>
+    <t>RemovedFromOrganization</t>
+  </si>
+  <si>
+    <t>MentionedOnCard</t>
+  </si>
+  <si>
+    <t>UnconfirmedInvitedToBoard</t>
+  </si>
+  <si>
+    <t>UnconfirmedInvitedToOrganization</t>
+  </si>
+  <si>
+    <t>MakeAdminOfOrganization</t>
+  </si>
+  <si>
+    <t>CardDueSoon</t>
+  </si>
+  <si>
+    <t>{0} commented on card {1}: '{2}'.</t>
+  </si>
+  <si>
+    <t>{0} made member {1} an admin of organization {2}.</t>
+  </si>
+  <si>
+    <t>{0} updated checkItem {1} on card {2}.</t>
+  </si>
+  <si>
+    <t>{0} mentioned you on card {1}: '{2}'.</t>
+  </si>
+  <si>
+    <t>{0} removed member {1} from organization {2}.</t>
+  </si>
+  <si>
+    <t>{0} removed you from card {1}.</t>
+  </si>
+  <si>
+    <t>{0} created card {1} on board {2}.</t>
+  </si>
+  <si>
+    <t>{0} closed board {1}.</t>
+  </si>
+  <si>
+    <t>{0} changed card {1}.</t>
+  </si>
+  <si>
+    <t>{0} assigned you to card {1}.</t>
+  </si>
+  <si>
+    <t>{0} added you to board {1}.</t>
+  </si>
+  <si>
+    <t>{0} added member {1} to board {2} as an admin.</t>
+  </si>
+  <si>
+    <t>{0} added member {1} to organization {2} as an admin.</t>
+  </si>
+  <si>
+    <t>n.GetString("attachment.name"), n.GetString("card.name")</t>
+  </si>
+  <si>
+    <t>n.GetString("board.name")</t>
+  </si>
+  <si>
+    <t>n.GetString("card.name")</t>
+  </si>
+  <si>
+    <t>n.Member.FullName, n.GetString("organization.name")</t>
+  </si>
+  <si>
+    <t>n.Member.FullName, n.GetString("card.name")</t>
+  </si>
+  <si>
+    <t>n.Member.FullName, n.GetString("board.name")</t>
+  </si>
+  <si>
+    <t>n.GetString("card.name"), n.GetString("text")</t>
+  </si>
+  <si>
+    <t>n.GetString("card.name"), n.GetString("board.name")</t>
+  </si>
+  <si>
+    <t>n.GetString("checkItem.name"), n.GetString("card.name")</t>
+  </si>
+  <si>
+    <t>Card {1} is due soon.</t>
+  </si>
+  <si>
+    <t>a.GetString("attachment.name"), a.GetString("card.name")</t>
+  </si>
+  <si>
+    <t>a.GetString("checklist.name"), a.GetString("card.name")</t>
+  </si>
+  <si>
+    <t>a.GetString("card.name"), a.GetString("text")</t>
+  </si>
+  <si>
+    <t>a.GetString("checkItem.name")</t>
+  </si>
+  <si>
+    <t>a.GetString("board.name"), a.GetString("boardSource.name")</t>
+  </si>
+  <si>
+    <t>a.GetString("card.name"), a.GetString("cardSource.name")</t>
+  </si>
+  <si>
+    <t>a.GetString("board.name")</t>
+  </si>
+  <si>
+    <t>a.GetString("card.name")</t>
+  </si>
+  <si>
+    <t>a.GetString("list.name")</t>
+  </si>
+  <si>
+    <t>a.GetString("organization.name")</t>
+  </si>
+  <si>
+    <t>a.GetString("card.idShort"), a.GetString("board.name")</t>
+  </si>
+  <si>
+    <t>a.Member.FullName, a.GetString("board.name")</t>
+  </si>
+  <si>
+    <t>a.Member.FullName, a.GetString("card.name")</t>
+  </si>
+  <si>
+    <t>a.GetString("board.id"), a.GetString("organization.name")</t>
+  </si>
+  <si>
+    <t>a.Member.FullName, a.GetString("organization.name")</t>
+  </si>
+  <si>
+    <t>a.GetString("board.name"), a.GetString("organization.name")</t>
+  </si>
+  <si>
+    <t>a.GetString("checklist.name")</t>
+  </si>
+  <si>
+    <t>a.GetString("card.name"), a.GetString("listBefore.name"), a.GetString("listAfter.name")</t>
+  </si>
+  <si>
+    <t>{0} commented on card #{1}: '{2}'.</t>
   </si>
 </sst>
 </file>
@@ -5933,15 +6072,16 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.42578125" customWidth="1"/>
-    <col min="4" max="4" width="86.140625" customWidth="1"/>
+    <col min="2" max="2" width="60" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="160" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -5952,7 +6092,7 @@
         <v>223</v>
       </c>
       <c r="C1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D1" t="s">
         <v>34</v>
@@ -5966,11 +6106,11 @@
         <v>269</v>
       </c>
       <c r="C2" t="s">
-        <v>313</v>
+        <v>357</v>
       </c>
       <c r="D2" t="str">
-        <f>"{ActionType."&amp;A2&amp;", a =&gt; string.Format("""&amp;B2&amp;""", a.MemberCreator, "&amp;C2&amp;")},"</f>
-        <v>{ActionType.AddAttachmentToCard, a =&gt; string.Format("{0} attached {1} to card {2}.", a.MemberCreator, a.Attachment, a.Card)},</v>
+        <f>"{ActionType."&amp;A2&amp;", a =&gt; a.ToString("""&amp;B2&amp;""", "&amp;C2&amp;")},"</f>
+        <v>{ActionType.AddAttachmentToCard, a =&gt; a.ToString("{0} attached {1} to card {2}.", a.GetString("attachment.name"), a.GetString("card.name"))},</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5981,11 +6121,11 @@
         <v>270</v>
       </c>
       <c r="C3" t="s">
-        <v>314</v>
+        <v>358</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D47" si="0">"{ActionType."&amp;A3&amp;", a =&gt; string.Format("""&amp;B3&amp;""", a.MemberCreator, "&amp;C3&amp;")},"</f>
-        <v>{ActionType.AddChecklistToCard, a =&gt; string.Format("{0} added checklist {1} to card {2}.", a.MemberCreator, a.CheckList, a.Card)},</v>
+        <f t="shared" ref="D3:D47" si="0">"{ActionType."&amp;A3&amp;", a =&gt; a.ToString("""&amp;B3&amp;""", "&amp;C3&amp;")},"</f>
+        <v>{ActionType.AddChecklistToCard, a =&gt; a.ToString("{0} added checklist {1} to card {2}.", a.GetString("checklist.name"), a.GetString("card.name"))},</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5996,11 +6136,11 @@
         <v>271</v>
       </c>
       <c r="C4" t="s">
-        <v>315</v>
+        <v>368</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.AddMemberToBoard, a =&gt; string.Format("{0} added member {1} to board {2}.", a.MemberCreator, a.Member, a.Board)},</v>
+        <v>{ActionType.AddMemberToBoard, a =&gt; a.ToString("{0} added member {1} to board {2}.", a.Member.FullName, a.GetString("board.name"))},</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6011,11 +6151,11 @@
         <v>272</v>
       </c>
       <c r="C5" t="s">
-        <v>316</v>
+        <v>369</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.AddMemberToCard, a =&gt; string.Format("{0} assigned member {1} to card {2}.", a.MemberCreator, a.Member, a.Card)},</v>
+        <v>{ActionType.AddMemberToCard, a =&gt; a.ToString("{0} assigned member {1} to card {2}.", a.Member.FullName, a.GetString("card.name"))},</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -6026,11 +6166,11 @@
         <v>273</v>
       </c>
       <c r="C6" t="s">
-        <v>317</v>
+        <v>371</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.AddMemberToOrganization, a =&gt; string.Format("{0} added member {1} to organization {2}.", a.MemberCreator, a.Member, a.Organization)},</v>
+        <v>{ActionType.AddMemberToOrganization, a =&gt; a.ToString("{0} added member {1} to organization {2}.", a.Member.FullName, a.GetString("organization.name"))},</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6041,11 +6181,11 @@
         <v>274</v>
       </c>
       <c r="C7" t="s">
-        <v>318</v>
+        <v>370</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.AddToOrganizationBoard, a =&gt; string.Format("{0} moved board {1} into organization {2}.", a.MemberCreator, a.Board, a.Organization)},</v>
+        <v>{ActionType.AddToOrganizationBoard, a =&gt; a.ToString("{0} moved board {1} into organization {2}.", a.GetString("board.id"), a.GetString("organization.name"))},</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6053,14 +6193,14 @@
         <v>230</v>
       </c>
       <c r="B8" t="s">
-        <v>275</v>
+        <v>375</v>
       </c>
       <c r="C8" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.CommentCard, a =&gt; string.Format("{0} commented on card {1}.", a.MemberCreator, a.Card)},</v>
+        <v>{ActionType.CommentCard, a =&gt; a.ToString("{0} commented on card #{1}: '{2}'.", a.GetString("card.name"), a.GetString("text"))},</v>
       </c>
     </row>
     <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -6069,7 +6209,7 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.CopyCommentCard, a =&gt; string.Format("", a.MemberCreator, )},</v>
+        <v>{ActionType.CopyCommentCard, a =&gt; a.ToString("", )},</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -6077,14 +6217,14 @@
         <v>232</v>
       </c>
       <c r="B10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C10" t="s">
-        <v>320</v>
+        <v>360</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.ConvertToCardFromCheckItem, a =&gt; string.Format("{0} converted checkitem {1} to a card.", a.MemberCreator, a.CheckItem)},</v>
+        <v>{ActionType.ConvertToCardFromCheckItem, a =&gt; a.ToString("{0} converted checkitem {1} to a card.", a.GetString("checkItem.name"))},</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -6092,14 +6232,14 @@
         <v>233</v>
       </c>
       <c r="B11" t="s">
-        <v>277</v>
+        <v>312</v>
       </c>
       <c r="C11" t="s">
-        <v>321</v>
+        <v>361</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.CopyBoard, a =&gt; string.Format("{0} created board {1} from board {2}.", a.MemberCreator, a.Board, a.SourceBoard)},</v>
+        <v>{ActionType.CopyBoard, a =&gt; a.ToString("{0} copied board {1} from board {2}.", a.GetString("board.name"), a.GetString("boardSource.name"))},</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -6107,14 +6247,14 @@
         <v>234</v>
       </c>
       <c r="B12" t="s">
-        <v>278</v>
+        <v>311</v>
       </c>
       <c r="C12" t="s">
-        <v>322</v>
+        <v>362</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.CopyCard, a =&gt; string.Format("{0} created card {1} from card {2}.", a.MemberCreator, a.Card, a.SourceCard)},</v>
+        <v>{ActionType.CopyCard, a =&gt; a.ToString("{0} copied card {1} from card {2}.", a.GetString("card.name"), a.GetString("cardSource.name"))},</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -6122,14 +6262,14 @@
         <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C13" t="s">
-        <v>323</v>
+        <v>363</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.CreateBoard, a =&gt; string.Format("{0} created board {1}.", a.MemberCreator, a.Board)},</v>
+        <v>{ActionType.CreateBoard, a =&gt; a.ToString("{0} created board {1}.", a.GetString("board.name"))},</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -6137,14 +6277,14 @@
         <v>235</v>
       </c>
       <c r="B14" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C14" t="s">
-        <v>319</v>
+        <v>364</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.CreateCard, a =&gt; string.Format("{0} created card {1}.", a.MemberCreator, a.Card)},</v>
+        <v>{ActionType.CreateCard, a =&gt; a.ToString("{0} created card {1}.", a.GetString("card.name"))},</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -6152,14 +6292,14 @@
         <v>236</v>
       </c>
       <c r="B15" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C15" t="s">
-        <v>324</v>
+        <v>365</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.CreateList, a =&gt; string.Format("{0} created list {1}.", a.MemberCreator, a.List)},</v>
+        <v>{ActionType.CreateList, a =&gt; a.ToString("{0} created list {1}.", a.GetString("list.name"))},</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -6167,14 +6307,14 @@
         <v>237</v>
       </c>
       <c r="B16" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C16" t="s">
-        <v>325</v>
+        <v>366</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.CreateOrganization, a =&gt; string.Format("{0} created organization {1}.", a.MemberCreator, a.Organization)},</v>
+        <v>{ActionType.CreateOrganization, a =&gt; a.ToString("{0} created organization {1}.", a.GetString("organization.name"))},</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -6182,14 +6322,14 @@
         <v>238</v>
       </c>
       <c r="B17" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C17" t="s">
-        <v>313</v>
+        <v>357</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.DeleteAttachmentFromCard, a =&gt; string.Format("{0} removed attachment {1} from card {2}.", a.MemberCreator, a.Attachment, a.Card)},</v>
+        <v>{ActionType.DeleteAttachmentFromCard, a =&gt; a.ToString("{0} removed attachment {1} from card {2}.", a.GetString("attachment.name"), a.GetString("card.name"))},</v>
       </c>
     </row>
     <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -6197,11 +6337,11 @@
         <v>239</v>
       </c>
       <c r="B18" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.DeleteBoardInvitation, a =&gt; string.Format("{0} rescinded an invitation to member {1} to join board {2}.", a.MemberCreator, )},</v>
+        <v>{ActionType.DeleteBoardInvitation, a =&gt; a.ToString("{0} rescinded an invitation to member {1} to join board {2}.", )},</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -6209,14 +6349,14 @@
         <v>240</v>
       </c>
       <c r="B19" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C19" t="s">
-        <v>326</v>
+        <v>367</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.DeleteCard, a =&gt; string.Format("{0} deleted card {1} from {2}.", a.MemberCreator, a.CardShortId, a.Board)},</v>
+        <v>{ActionType.DeleteCard, a =&gt; a.ToString("{0} deleted card {1} from {2}.", a.GetString("card.idShort"), a.GetString("board.name"))},</v>
       </c>
     </row>
     <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -6224,11 +6364,11 @@
         <v>241</v>
       </c>
       <c r="B20" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.DeleteOrganizationInvitation, a =&gt; string.Format("{0} rescinded an invitation to member {1} to join organization {2}.", a.MemberCreator, )},</v>
+        <v>{ActionType.DeleteOrganizationInvitation, a =&gt; a.ToString("{0} rescinded an invitation to member {1} to join organization {2}.", )},</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -6236,14 +6376,14 @@
         <v>242</v>
       </c>
       <c r="B21" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C21" t="s">
-        <v>315</v>
+        <v>368</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.MakeAdminOfBoard, a =&gt; string.Format("{0} made member {1} an admin of board {2}.", a.MemberCreator, a.Member, a.Board)},</v>
+        <v>{ActionType.MakeAdminOfBoard, a =&gt; a.ToString("{0} made member {1} an admin of board {2}.", a.Member.FullName, a.GetString("board.name"))},</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -6251,14 +6391,14 @@
         <v>243</v>
       </c>
       <c r="B22" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C22" t="s">
-        <v>315</v>
+        <v>368</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.MakeNormalMemberOfBoard, a =&gt; string.Format("{0} made member {1} a normal user of board {2}.", a.MemberCreator, a.Member, a.Board)},</v>
+        <v>{ActionType.MakeNormalMemberOfBoard, a =&gt; a.ToString("{0} made member {1} a normal user of board {2}.", a.Member.FullName, a.GetString("board.name"))},</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -6266,14 +6406,14 @@
         <v>244</v>
       </c>
       <c r="B23" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C23" t="s">
-        <v>317</v>
+        <v>371</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.MakeNormalMemberOfOrganization, a =&gt; string.Format("{0} made member {1} a normal user of organization {2}.", a.MemberCreator, a.Member, a.Organization)},</v>
+        <v>{ActionType.MakeNormalMemberOfOrganization, a =&gt; a.ToString("{0} made member {1} a normal user of organization {2}.", a.Member.FullName, a.GetString("organization.name"))},</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -6281,29 +6421,26 @@
         <v>245</v>
       </c>
       <c r="B24" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C24" t="s">
-        <v>315</v>
+        <v>368</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.MakeObserverOfBoard, a =&gt; string.Format("{0} made member {1} an observer of board {2}.", a.MemberCreator, a.Member, a.Board)},</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>{ActionType.MakeObserverOfBoard, a =&gt; a.ToString("{0} made member {1} an observer of board {2}.", a.Member.FullName, a.GetString("board.name"))},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>246</v>
       </c>
       <c r="B25" t="s">
-        <v>290</v>
-      </c>
-      <c r="C25" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
       <c r="D25" t="str">
-        <f>"{ActionType."&amp;A25&amp;", a =&gt; string.Format("""&amp;B25&amp;""", a.MemberCreator, "&amp;C25&amp;")},"</f>
-        <v>{ActionType.MemberJoinedTrello, a =&gt; string.Format("Three cheers for {0}: the newest member of Trello!", a.MemberCreator, None)},</v>
+        <f t="shared" si="0"/>
+        <v>{ActionType.MemberJoinedTrello, a =&gt; a.ToString("Three cheers for {0}: the newest member of Trello!", )},</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -6311,14 +6448,14 @@
         <v>247</v>
       </c>
       <c r="B26" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C26" t="s">
-        <v>319</v>
+        <v>364</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.MoveCardFromBoard, a =&gt; string.Format("{0} moved card {1} from board {2} to board {3}.", a.MemberCreator, a.Card)},</v>
+        <v>{ActionType.MoveCardFromBoard, a =&gt; a.ToString("{0} moved card {1} from board {2} to board {3}.", a.GetString("card.name"))},</v>
       </c>
     </row>
     <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -6326,11 +6463,11 @@
         <v>248</v>
       </c>
       <c r="B27" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.MoveListFromBoard, a =&gt; string.Format("{0} moved list {1} from board {2} to board {3}.", a.MemberCreator, )},</v>
+        <v>{ActionType.MoveListFromBoard, a =&gt; a.ToString("{0} moved list {1} from board {2} to board {3}.", )},</v>
       </c>
     </row>
     <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -6338,11 +6475,11 @@
         <v>249</v>
       </c>
       <c r="B28" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.MoveCardToBoard, a =&gt; string.Format("{0} moved card {1} from board {2} to board {3}.", a.MemberCreator, )},</v>
+        <v>{ActionType.MoveCardToBoard, a =&gt; a.ToString("{0} moved card {1} from board {2} to board {3}.", )},</v>
       </c>
     </row>
     <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -6350,11 +6487,11 @@
         <v>250</v>
       </c>
       <c r="B29" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.MoveListToBoard, a =&gt; string.Format("{0} moved list {1} from board {2} to board {3}.", a.MemberCreator, )},</v>
+        <v>{ActionType.MoveListToBoard, a =&gt; a.ToString("{0} moved list {1} from board {2} to board {3}.", )},</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -6362,14 +6499,14 @@
         <v>251</v>
       </c>
       <c r="B30" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C30" t="s">
-        <v>315</v>
+        <v>368</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.RemoveAdminFromBoard, a =&gt; string.Format("{0} removed member {1} as an admin of board {2}.", a.MemberCreator, a.Member, a.Board)},</v>
+        <v>{ActionType.RemoveAdminFromBoard, a =&gt; a.ToString("{0} removed member {1} as an admin of board {2}.", a.Member.FullName, a.GetString("board.name"))},</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -6377,14 +6514,14 @@
         <v>252</v>
       </c>
       <c r="B31" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C31" t="s">
-        <v>317</v>
+        <v>371</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.RemoveAdminFromOrganization, a =&gt; string.Format("{0} removed member {1} as an admin of organization {2}.", a.MemberCreator, a.Member, a.Organization)},</v>
+        <v>{ActionType.RemoveAdminFromOrganization, a =&gt; a.ToString("{0} removed member {1} as an admin of organization {2}.", a.Member.FullName, a.GetString("organization.name"))},</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -6392,14 +6529,14 @@
         <v>253</v>
       </c>
       <c r="B32" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C32" t="s">
-        <v>314</v>
+        <v>358</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.RemoveChecklistFromCard, a =&gt; string.Format("{0} deleted checklist {1} from card {2}.", a.MemberCreator, a.CheckList, a.Card)},</v>
+        <v>{ActionType.RemoveChecklistFromCard, a =&gt; a.ToString("{0} deleted checklist {1} from card {2}.", a.GetString("checklist.name"), a.GetString("card.name"))},</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -6407,14 +6544,14 @@
         <v>254</v>
       </c>
       <c r="B33" t="s">
-        <v>329</v>
+        <v>310</v>
       </c>
       <c r="C33" t="s">
-        <v>318</v>
+        <v>372</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.RemoveFromOrganizationBoard, a =&gt; string.Format("{0} removed board {1} from organization {2}.", a.MemberCreator, a.Board, a.Organization)},</v>
+        <v>{ActionType.RemoveFromOrganizationBoard, a =&gt; a.ToString("{0} removed board {1} from organization {2}.", a.GetString("board.name"), a.GetString("organization.name"))},</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -6422,14 +6559,14 @@
         <v>255</v>
       </c>
       <c r="B34" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C34" t="s">
-        <v>315</v>
+        <v>368</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.RemoveMemberFromBoard, a =&gt; string.Format("{0} removed member {1} from board {2}.", a.MemberCreator, a.Member, a.Board)},</v>
+        <v>{ActionType.RemoveMemberFromBoard, a =&gt; a.ToString("{0} removed member {1} from board {2}.", a.Member.FullName, a.GetString("board.name"))},</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -6437,14 +6574,14 @@
         <v>256</v>
       </c>
       <c r="B35" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C35" t="s">
-        <v>316</v>
+        <v>369</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.RemoveMemberFromCard, a =&gt; string.Format("{0} removed member {1} from card {2}.", a.MemberCreator, a.Member, a.Card)},</v>
+        <v>{ActionType.RemoveMemberFromCard, a =&gt; a.ToString("{0} removed member {1} from card {2}.", a.Member.FullName, a.GetString("card.name"))},</v>
       </c>
     </row>
     <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -6452,11 +6589,11 @@
         <v>257</v>
       </c>
       <c r="B36" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.UnconfirmedBoardInvitation, a =&gt; string.Format("{0} invited Trello outsider {1} to join the board.", a.MemberCreator, )},</v>
+        <v>{ActionType.UnconfirmedBoardInvitation, a =&gt; a.ToString("{0} invited Trello outsider {1} to join the board.", )},</v>
       </c>
     </row>
     <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -6464,11 +6601,11 @@
         <v>258</v>
       </c>
       <c r="B37" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.UnconfirmedOrganizationInvitation, a =&gt; string.Format("{0} invited Trello outsider {1} to join the organization.", a.MemberCreator, )},</v>
+        <v>{ActionType.UnconfirmedOrganizationInvitation, a =&gt; a.ToString("{0} invited Trello outsider {1} to join the organization.", )},</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -6476,14 +6613,14 @@
         <v>259</v>
       </c>
       <c r="B38" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C38" t="s">
-        <v>323</v>
+        <v>363</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.UpdateBoard, a =&gt; string.Format("{0} updated board {1}.", a.MemberCreator, a.Board)},</v>
+        <v>{ActionType.UpdateBoard, a =&gt; a.ToString("{0} updated board {1}.", a.GetString("board.name"))},</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -6491,14 +6628,14 @@
         <v>260</v>
       </c>
       <c r="B39" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C39" t="s">
-        <v>319</v>
+        <v>364</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.UpdateCard, a =&gt; string.Format("{0} updated card {1}.", a.MemberCreator, a.Card)},</v>
+        <v>{ActionType.UpdateCard, a =&gt; a.ToString("{0} updated card {1}.", a.GetString("card.name"))},</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -6506,14 +6643,14 @@
         <v>261</v>
       </c>
       <c r="B40" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C40" t="s">
-        <v>320</v>
+        <v>360</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.UpdateCheckItemStateOnCard, a =&gt; string.Format("{0} updated checkitem {1}.", a.MemberCreator, a.CheckItem)},</v>
+        <v>{ActionType.UpdateCheckItemStateOnCard, a =&gt; a.ToString("{0} updated checkitem {1}.", a.GetString("checkItem.name"))},</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -6521,14 +6658,14 @@
         <v>262</v>
       </c>
       <c r="B41" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C41" t="s">
-        <v>327</v>
+        <v>373</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.UpdateChecklist, a =&gt; string.Format("{0} updated checklist {1}.", a.MemberCreator, a.CheckList)},</v>
+        <v>{ActionType.UpdateChecklist, a =&gt; a.ToString("{0} updated checklist {1}.", a.GetString("checklist.name"))},</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -6536,14 +6673,14 @@
         <v>263</v>
       </c>
       <c r="B42" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C42" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D42" t="str">
-        <f t="shared" si="0"/>
-        <v>{ActionType.UpdateMember, a =&gt; string.Format("{0} updated their profile.", a.MemberCreator, None)},</v>
+        <f>"{ActionType."&amp;A42&amp;", a =&gt; a.ToString("""&amp;B42&amp;""")},"</f>
+        <v>{ActionType.UpdateMember, a =&gt; a.ToString("{0} updated their profile.")},</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -6551,14 +6688,14 @@
         <v>264</v>
       </c>
       <c r="B43" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C43" t="s">
-        <v>325</v>
+        <v>366</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.UpdateOrganization, a =&gt; string.Format("{0} updated organization {1}.", a.MemberCreator, a.Organization)},</v>
+        <v>{ActionType.UpdateOrganization, a =&gt; a.ToString("{0} updated organization {1}.", a.GetString("organization.name"))},</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -6566,14 +6703,14 @@
         <v>265</v>
       </c>
       <c r="B44" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C44" t="s">
-        <v>328</v>
+        <v>374</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.UpdateCardIdList, a =&gt; string.Format("{0} moved card {1} from list {2} to list {3}.", a.MemberCreator, a.Card, a.ListBefore, a.ListAfter)},</v>
+        <v>{ActionType.UpdateCardIdList, a =&gt; a.ToString("{0} moved card {1} from list {2} to list {3}.", a.GetString("card.name"), a.GetString("listBefore.name"), a.GetString("listAfter.name"))},</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -6581,14 +6718,14 @@
         <v>266</v>
       </c>
       <c r="B45" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C45" t="s">
-        <v>319</v>
+        <v>364</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.UpdateCardClosed, a =&gt; string.Format("{0} archived card {1}.", a.MemberCreator, a.Card)},</v>
+        <v>{ActionType.UpdateCardClosed, a =&gt; a.ToString("{0} archived card {1}.", a.GetString("card.name"))},</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -6596,14 +6733,14 @@
         <v>267</v>
       </c>
       <c r="B46" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C46" t="s">
-        <v>319</v>
+        <v>364</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.UpdateCardDesc, a =&gt; string.Format("{0} changed the description of card {1}.", a.MemberCreator, a.Card)},</v>
+        <v>{ActionType.UpdateCardDesc, a =&gt; a.ToString("{0} changed the description of card {1}.", a.GetString("card.name"))},</v>
       </c>
     </row>
     <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -6611,11 +6748,11 @@
         <v>268</v>
       </c>
       <c r="B47" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
-        <v>{ActionType.UpdateCardName, a =&gt; string.Format("{0} changed the name of card {1} to {2}.", a.MemberCreator, )},</v>
+        <v>{ActionType.UpdateCardName, a =&gt; a.ToString("{0} changed the name of card {1} to {2}.", )},</v>
       </c>
     </row>
   </sheetData>
@@ -6633,12 +6770,373 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.28515625" customWidth="1"/>
+    <col min="4" max="4" width="145.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D12" si="0">"{NotificationType."&amp;A2&amp;", n =&gt; n.ToString("""&amp;B2&amp;""", "&amp;C2&amp;")},"</f>
+        <v>{NotificationType.AddedAttachmentToCard, n =&gt; n.ToString("{0} attached {1} to card {2}.", n.GetString("attachment.name"), n.GetString("card.name"))},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B3" t="s">
+        <v>344</v>
+      </c>
+      <c r="C3" t="s">
+        <v>348</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>{NotificationType.AddedToBoard, n =&gt; n.ToString("{0} added you to board {1}.", n.GetString("board.name"))},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B4" t="s">
+        <v>343</v>
+      </c>
+      <c r="C4" t="s">
+        <v>349</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>{NotificationType.AddedToCard, n =&gt; n.ToString("{0} assigned you to card {1}.", n.GetString("card.name"))},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>{NotificationType.AddedToOrganization, n =&gt; n.ToString("{0} added member {1} to organization {2}.", n.Member.FullName, n.GetString("organization.name"))},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>317</v>
+      </c>
+      <c r="B6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>{NotificationType.AddedMemberToCard, n =&gt; n.ToString("{0} assigned member {1} to card {2}.", n.Member.FullName, n.GetString("card.name"))},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>318</v>
+      </c>
+      <c r="B7" t="s">
+        <v>345</v>
+      </c>
+      <c r="C7" t="s">
+        <v>352</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>{NotificationType.AddAdminToBoard, n =&gt; n.ToString("{0} added member {1} to board {2} as an admin.", n.Member.FullName, n.GetString("board.name"))},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>319</v>
+      </c>
+      <c r="B8" t="s">
+        <v>346</v>
+      </c>
+      <c r="C8" t="s">
+        <v>350</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>{NotificationType.AddAdminToOrganization, n =&gt; n.ToString("{0} added member {1} to organization {2} as an admin.", n.Member.FullName, n.GetString("organization.name"))},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>320</v>
+      </c>
+      <c r="B9" t="s">
+        <v>342</v>
+      </c>
+      <c r="C9" t="s">
+        <v>349</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>{NotificationType.ChangeCard, n =&gt; n.ToString("{0} changed card {1}.", n.GetString("card.name"))},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>321</v>
+      </c>
+      <c r="B10" t="s">
+        <v>341</v>
+      </c>
+      <c r="C10" t="s">
+        <v>348</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>{NotificationType.CloseBoard, n =&gt; n.ToString("{0} closed board {1}.", n.GetString("board.name"))},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B11" t="s">
+        <v>334</v>
+      </c>
+      <c r="C11" t="s">
+        <v>353</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>{NotificationType.CommentCard, n =&gt; n.ToString("{0} commented on card {1}: '{2}'.", n.GetString("card.name"), n.GetString("text"))},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>322</v>
+      </c>
+      <c r="B12" t="s">
+        <v>340</v>
+      </c>
+      <c r="C12" t="s">
+        <v>354</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>{NotificationType.CreatedCard, n =&gt; n.ToString("{0} created card {1} on board {2}.", n.GetString("card.name"), n.GetString("board.name"))},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>323</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" ref="D3:D24" si="1">"{NotificationType."&amp;A13&amp;", n =&gt; string.Format("""&amp;B13&amp;""", n.MemberCreator, "&amp;C13&amp;")},"</f>
+        <v>{NotificationType.InvitedToBoard, n =&gt; string.Format("", n.MemberCreator, )},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>324</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>{NotificationType.InvitedToOrganization, n =&gt; string.Format("", n.MemberCreator, )},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>325</v>
+      </c>
+      <c r="B15" t="s">
+        <v>293</v>
+      </c>
+      <c r="C15" t="s">
+        <v>352</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" ref="D15:D19" si="2">"{NotificationType."&amp;A15&amp;", n =&gt; n.ToString("""&amp;B15&amp;""", "&amp;C15&amp;")},"</f>
+        <v>{NotificationType.RemovedFromBoard, n =&gt; n.ToString("{0} removed member {1} from board {2}.", n.Member.FullName, n.GetString("board.name"))},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>326</v>
+      </c>
+      <c r="B16" t="s">
+        <v>339</v>
+      </c>
+      <c r="C16" t="s">
+        <v>349</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>{NotificationType.RemovedFromCard, n =&gt; n.ToString("{0} removed you from card {1}.", n.GetString("card.name"))},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>327</v>
+      </c>
+      <c r="B17" t="s">
+        <v>338</v>
+      </c>
+      <c r="C17" t="s">
+        <v>350</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="2"/>
+        <v>{NotificationType.RemovedMemberFromCard, n =&gt; n.ToString("{0} removed member {1} from organization {2}.", n.Member.FullName, n.GetString("organization.name"))},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>328</v>
+      </c>
+      <c r="B18" t="s">
+        <v>338</v>
+      </c>
+      <c r="C18" t="s">
+        <v>350</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="2"/>
+        <v>{NotificationType.RemovedFromOrganization, n =&gt; n.ToString("{0} removed member {1} from organization {2}.", n.Member.FullName, n.GetString("organization.name"))},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>329</v>
+      </c>
+      <c r="B19" t="s">
+        <v>337</v>
+      </c>
+      <c r="C19" t="s">
+        <v>353</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="2"/>
+        <v>{NotificationType.MentionedOnCard, n =&gt; n.ToString("{0} mentioned you on card {1}: '{2}'.", n.GetString("card.name"), n.GetString("text"))},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>330</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>{NotificationType.UnconfirmedInvitedToBoard, n =&gt; string.Format("", n.MemberCreator, )},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>331</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>{NotificationType.UnconfirmedInvitedToOrganization, n =&gt; string.Format("", n.MemberCreator, )},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>261</v>
+      </c>
+      <c r="B22" t="s">
+        <v>336</v>
+      </c>
+      <c r="C22" t="s">
+        <v>355</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" ref="D22:D24" si="3">"{NotificationType."&amp;A22&amp;", n =&gt; n.ToString("""&amp;B22&amp;""", "&amp;C22&amp;")},"</f>
+        <v>{NotificationType.UpdateCheckItemStateOnCard, n =&gt; n.ToString("{0} updated checkItem {1} on card {2}.", n.GetString("checkItem.name"), n.GetString("card.name"))},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>242</v>
+      </c>
+      <c r="B23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C23" t="s">
+        <v>352</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="3"/>
+        <v>{NotificationType.MakeAdminOfBoard, n =&gt; n.ToString("{0} made member {1} an admin of board {2}.", n.Member.FullName, n.GetString("board.name"))},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>332</v>
+      </c>
+      <c r="B24" t="s">
+        <v>335</v>
+      </c>
+      <c r="C24" t="s">
+        <v>350</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="3"/>
+        <v>{NotificationType.MakeAdminOfOrganization, n =&gt; n.ToString("{0} made member {1} an admin of organization {2}.", n.Member.FullName, n.GetString("organization.name"))},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>333</v>
+      </c>
+      <c r="B25" t="s">
+        <v>356</v>
+      </c>
+      <c r="C25" t="s">
+        <v>349</v>
+      </c>
+      <c r="D25" t="str">
+        <f>"{NotificationType."&amp;A25&amp;", n =&gt; n.ToString("""&amp;B25&amp;""", "&amp;C25&amp;")},"</f>
+        <v>{NotificationType.CardDueSoon, n =&gt; n.ToString("Card {1} is due soon.", n.GetString("card.name"))},</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D25"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BUG FIX: ExpiringList throwing NullReferenceException when using extension methods Added Member.OneTimeMessagesDismissed. Replaced Member.PinnedBoards with Member.StarredBoards.
</commit_message>
<xml_diff>
--- a/Endpoint definitions.xlsx
+++ b/Endpoint definitions.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="385">
   <si>
     <t>Entity</t>
   </si>
@@ -1169,9 +1169,6 @@
     <t>CallbackUrl</t>
   </si>
   <si>
-    <t>PinnedBoards</t>
-  </si>
-  <si>
     <t>Organizations</t>
   </si>
   <si>
@@ -1182,6 +1179,12 @@
   </si>
   <si>
     <t>"webhooks"</t>
+  </si>
+  <si>
+    <t>StarredBoards</t>
+  </si>
+  <si>
+    <t>"members","_id","boardStars"</t>
   </si>
 </sst>
 </file>
@@ -1256,8 +1259,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H164" totalsRowShown="0">
   <autoFilter ref="A1:H164"/>
-  <sortState ref="A2:H163">
-    <sortCondition ref="A1:A163"/>
+  <sortState ref="A2:H165">
+    <sortCondition ref="A1:A165"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" name="Entity"/>
@@ -1545,8 +1548,8 @@
   <dimension ref="A1:H164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A162" sqref="A162:XFD162"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A113" sqref="A113:XFD113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,28 +1594,28 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="str">
-        <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Action_Read_Refresh</v>
-      </c>
-      <c r="E2" t="str">
-        <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Action_Read_Refresh,</v>
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
+        <v>Action_Write_Delete</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
+        <v>Action_Write_Delete,</v>
       </c>
       <c r="F2" t="s">
         <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H2" t="str">
-        <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Action_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"actions","_id"})},</v>
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="str">
+        <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
+        <v>{EntityRequestType.Action_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"actions","_id"})},</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1620,28 +1623,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Action_Write_Delete</v>
-      </c>
-      <c r="E3" s="1" t="str">
-        <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Action_Write_Delete,</v>
+        <v>4</v>
+      </c>
+      <c r="D3" t="str">
+        <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
+        <v>Action_Read_Refresh</v>
+      </c>
+      <c r="E3" t="str">
+        <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
+        <v>Action_Read_Refresh,</v>
       </c>
       <c r="F3" t="s">
         <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="1" t="str">
-        <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Action_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"actions","_id"})},</v>
+        <v>168</v>
+      </c>
+      <c r="H3" t="str">
+        <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
+        <v>{EntityRequestType.Action_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"actions","_id"})},</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1649,28 +1652,28 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Attachment_Read_Refresh</v>
+        <v>Attachment_Write_Delete</v>
       </c>
       <c r="E4" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Attachment_Read_Refresh,</v>
+        <v>Attachment_Write_Delete,</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>101</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>168</v>
+        <v>17</v>
       </c>
       <c r="H4" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Attachment_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_cardId","attachments","_id"})},</v>
+        <v>{EntityRequestType.Attachment_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"cards","_cardId","attachments","_id"})},</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1678,28 +1681,28 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Attachment_Write_Delete</v>
+        <v>Attachment_Read_Refresh</v>
       </c>
       <c r="E5" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Attachment_Write_Delete,</v>
+        <v>Attachment_Read_Refresh,</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>101</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
+        <v>168</v>
       </c>
       <c r="H5" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Attachment_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"cards","_cardId","attachments","_id"})},</v>
+        <v>{EntityRequestType.Attachment_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_cardId","attachments","_id"})},</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1765,28 +1768,28 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Read_Cards</v>
+        <v>Board_Write_AddList</v>
       </c>
       <c r="E8" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Read_Cards,</v>
+        <v>Board_Write_AddList,</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>184</v>
+        <v>103</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H8" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Read_Cards, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_id","cards"})},</v>
+        <v>{EntityRequestType.Board_Write_AddList, () =&gt; new Endpoint(RestMethod.Post, new[]{"lists"})},</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1794,28 +1797,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>179</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Read_Checklists</v>
+        <v>Board_Write_AddOrUpdateMember</v>
       </c>
       <c r="E9" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Read_Checklists,</v>
+        <v>Board_Write_AddOrUpdateMember,</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>180</v>
+        <v>104</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H9" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Read_Checklists, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_id","checklists"})},</v>
+        <v>{EntityRequestType.Board_Write_AddOrUpdateMember, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_id","members"})},</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1826,25 +1829,25 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D10" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Read_InvitedMembers</v>
+        <v>Board_Read_Cards</v>
       </c>
       <c r="E10" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Read_InvitedMembers,</v>
+        <v>Board_Read_Cards,</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H10" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Read_InvitedMembers, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_id","membersInvited"})},</v>
+        <v>{EntityRequestType.Board_Read_Cards, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_id","cards"})},</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1855,25 +1858,25 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D11" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Read_Lists</v>
+        <v>Board_Read_Checklists</v>
       </c>
       <c r="E11" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Read_Lists,</v>
+        <v>Board_Read_Checklists,</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H11" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Read_Lists, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_id","lists"})},</v>
+        <v>{EntityRequestType.Board_Read_Checklists, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_id","checklists"})},</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1881,28 +1884,28 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>175</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Read_Members</v>
+        <v>Board_Write_Description</v>
       </c>
       <c r="E12" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Read_Members,</v>
+        <v>Board_Write_Description,</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H12" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Read_Members, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_id","members"})},</v>
+        <v>{EntityRequestType.Board_Write_Description, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_id"})},</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1913,25 +1916,25 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D13" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Read_Memberships</v>
+        <v>Board_Read_InvitedMembers</v>
       </c>
       <c r="E13" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Read_Memberships,</v>
+        <v>Board_Read_InvitedMembers,</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H13" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Read_Memberships, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_id","memberships"})},</v>
+        <v>{EntityRequestType.Board_Read_InvitedMembers, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_id","membersInvited"})},</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1939,28 +1942,28 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D14" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Read_Refresh</v>
+        <v>Board_Write_InviteMember</v>
       </c>
       <c r="E14" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Read_Refresh,</v>
+        <v>Board_Write_InviteMember,</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H14" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_id"})},</v>
+        <v>{EntityRequestType.Board_Write_InviteMember, () =&gt; new Endpoint(RestMethod.Post, new[]{string.Empty})},</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1971,25 +1974,25 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D15" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Write_AddList</v>
+        <v>Board_Write_IsClosed</v>
       </c>
       <c r="E15" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Write_AddList,</v>
+        <v>Board_Write_IsClosed,</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H15" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Write_AddList, () =&gt; new Endpoint(RestMethod.Post, new[]{"lists"})},</v>
+        <v>{EntityRequestType.Board_Write_IsClosed, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_id"})},</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2000,25 +2003,25 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D16" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Write_AddOrUpdateMember</v>
+        <v>Board_Write_IsPinned</v>
       </c>
       <c r="E16" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Write_AddOrUpdateMember,</v>
+        <v>Board_Write_IsPinned,</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>171</v>
       </c>
       <c r="H16" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Write_AddOrUpdateMember, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_id","members"})},</v>
+        <v>{EntityRequestType.Board_Write_IsPinned, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_id"})},</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2029,15 +2032,15 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Write_Description</v>
+        <v>Board_Write_IsSubscribed</v>
       </c>
       <c r="E17" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Write_Description,</v>
+        <v>Board_Write_IsSubscribed,</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>33</v>
@@ -2047,7 +2050,7 @@
       </c>
       <c r="H17" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Write_Description, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_id"})},</v>
+        <v>{EntityRequestType.Board_Write_IsSubscribed, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_id"})},</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2055,28 +2058,28 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>173</v>
       </c>
       <c r="D18" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Write_InviteMember</v>
+        <v>Board_Read_Lists</v>
       </c>
       <c r="E18" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Write_InviteMember,</v>
+        <v>Board_Read_Lists,</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>107</v>
+        <v>185</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H18" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Write_InviteMember, () =&gt; new Endpoint(RestMethod.Post, new[]{string.Empty})},</v>
+        <v>{EntityRequestType.Board_Read_Lists, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_id","lists"})},</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2087,25 +2090,25 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D19" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Write_IsClosed</v>
+        <v>Board_Write_MarkAsViewed</v>
       </c>
       <c r="E19" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Write_IsClosed,</v>
+        <v>Board_Write_MarkAsViewed,</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H19" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Write_IsClosed, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_id"})},</v>
+        <v>{EntityRequestType.Board_Write_MarkAsViewed, () =&gt; new Endpoint(RestMethod.Post, new[]{"boards","_id","markAsViewed"})},</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2113,28 +2116,28 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>175</v>
       </c>
       <c r="D20" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Write_IsPinned</v>
+        <v>Board_Read_Members</v>
       </c>
       <c r="E20" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Write_IsPinned,</v>
+        <v>Board_Read_Members,</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>33</v>
+        <v>104</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H20" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Write_IsPinned, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_id"})},</v>
+        <v>{EntityRequestType.Board_Read_Members, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_id","members"})},</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2142,28 +2145,28 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>176</v>
       </c>
       <c r="D21" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Write_IsSubscribed</v>
+        <v>Board_Read_Memberships</v>
       </c>
       <c r="E21" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Write_IsSubscribed,</v>
+        <v>Board_Read_Memberships,</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>33</v>
+        <v>183</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H21" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Write_IsSubscribed, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_id"})},</v>
+        <v>{EntityRequestType.Board_Read_Memberships, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_id","memberships"})},</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2174,25 +2177,25 @@
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Write_MarkAsViewed</v>
+        <v>Board_Write_Name</v>
       </c>
       <c r="E22" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Write_MarkAsViewed,</v>
+        <v>Board_Write_Name,</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>105</v>
+        <v>33</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H22" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Write_MarkAsViewed, () =&gt; new Endpoint(RestMethod.Post, new[]{"boards","_id","markAsViewed"})},</v>
+        <v>{EntityRequestType.Board_Write_Name, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_id"})},</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2203,15 +2206,15 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D23" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Write_Name</v>
+        <v>Board_Write_Organization</v>
       </c>
       <c r="E23" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Write_Name,</v>
+        <v>Board_Write_Organization,</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>33</v>
@@ -2221,7 +2224,7 @@
       </c>
       <c r="H23" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Write_Name, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_id"})},</v>
+        <v>{EntityRequestType.Board_Write_Organization, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_id"})},</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2229,28 +2232,28 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Board_Write_Organization</v>
+        <v>Board_Read_Refresh</v>
       </c>
       <c r="E24" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Board_Write_Organization,</v>
+        <v>Board_Read_Refresh,</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H24" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Board_Write_Organization, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_id"})},</v>
+        <v>{EntityRequestType.Board_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_id"})},</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2519,28 +2522,28 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D34" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>BoardPreferences_Read_Refresh</v>
+        <v>BoardPreferences_Write_AllowsSelfJoin</v>
       </c>
       <c r="E34" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>BoardPreferences_Read_Refresh,</v>
+        <v>BoardPreferences_Write_AllowsSelfJoin,</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H34" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.BoardPreferences_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_boardId","prefs"})},</v>
+        <v>{EntityRequestType.BoardPreferences_Write_AllowsSelfJoin, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_boardId","prefs","selfJoin"})},</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2551,25 +2554,25 @@
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D35" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>BoardPreferences_Write_AllowsSelfJoin</v>
+        <v>BoardPreferences_Write_Comments</v>
       </c>
       <c r="E35" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>BoardPreferences_Write_AllowsSelfJoin,</v>
+        <v>BoardPreferences_Write_Comments,</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>171</v>
       </c>
       <c r="H35" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.BoardPreferences_Write_AllowsSelfJoin, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_boardId","prefs","selfJoin"})},</v>
+        <v>{EntityRequestType.BoardPreferences_Write_Comments, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_boardId","prefs","comments"})},</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2580,25 +2583,25 @@
         <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D36" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>BoardPreferences_Write_Comments</v>
+        <v>BoardPreferences_Write_Invitations</v>
       </c>
       <c r="E36" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>BoardPreferences_Write_Comments,</v>
+        <v>BoardPreferences_Write_Invitations,</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>171</v>
       </c>
       <c r="H36" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.BoardPreferences_Write_Comments, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_boardId","prefs","comments"})},</v>
+        <v>{EntityRequestType.BoardPreferences_Write_Invitations, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_boardId","prefs","invitations"})},</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2609,25 +2612,25 @@
         <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D37" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>BoardPreferences_Write_Invitations</v>
+        <v>BoardPreferences_Write_PermissionLevel</v>
       </c>
       <c r="E37" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>BoardPreferences_Write_Invitations,</v>
+        <v>BoardPreferences_Write_PermissionLevel,</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>171</v>
       </c>
       <c r="H37" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.BoardPreferences_Write_Invitations, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_boardId","prefs","invitations"})},</v>
+        <v>{EntityRequestType.BoardPreferences_Write_PermissionLevel, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_boardId","prefs","permissionLevel"})},</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2635,28 +2638,28 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="D38" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>BoardPreferences_Write_PermissionLevel</v>
+        <v>BoardPreferences_Read_Refresh</v>
       </c>
       <c r="E38" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>BoardPreferences_Write_PermissionLevel,</v>
+        <v>BoardPreferences_Read_Refresh,</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H38" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.BoardPreferences_Write_PermissionLevel, () =&gt; new Endpoint(RestMethod.Put, new[]{"boards","_boardId","prefs","permissionLevel"})},</v>
+        <v>{EntityRequestType.BoardPreferences_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"boards","_boardId","prefs"})},</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2751,28 +2754,28 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>188</v>
+        <v>47</v>
       </c>
       <c r="D42" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Read_Attachments</v>
+        <v>Card_Write_AddAttachment</v>
       </c>
       <c r="E42" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Read_Attachments,</v>
+        <v>Card_Write_AddAttachment,</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>121</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H42" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Read_Attachments, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_id","attachments"})},</v>
+        <v>{EntityRequestType.Card_Write_AddAttachment, () =&gt; new Endpoint(RestMethod.Post, new[]{"cards","_id","attachments"})},</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2780,28 +2783,28 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>191</v>
+        <v>48</v>
       </c>
       <c r="D43" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Read_CheckItems</v>
+        <v>Card_Write_AddChecklist</v>
       </c>
       <c r="E43" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Read_CheckItems,</v>
+        <v>Card_Write_AddChecklist,</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H43" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Read_CheckItems, () =&gt; new Endpoint(RestMethod.Get, new[]{"checklists","_id","checkItems"})},</v>
+        <v>{EntityRequestType.Card_Write_AddChecklist, () =&gt; new Endpoint(RestMethod.Post, new[]{"checklists"})},</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -2809,28 +2812,28 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>382</v>
+        <v>49</v>
       </c>
       <c r="D44" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Read_CheckLists</v>
+        <v>Card_Write_AddComment</v>
       </c>
       <c r="E44" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Read_CheckLists,</v>
+        <v>Card_Write_AddComment,</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>189</v>
+        <v>123</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H44" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Read_CheckLists, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_id","checklists"})},</v>
+        <v>{EntityRequestType.Card_Write_AddComment, () =&gt; new Endpoint(RestMethod.Post, new[]{"cards","_id","actions","comments"})},</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2838,28 +2841,28 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>213</v>
+        <v>50</v>
       </c>
       <c r="D45" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Read_Labels</v>
+        <v>Card_Write_ApplyLabel</v>
       </c>
       <c r="E45" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Read_Labels,</v>
+        <v>Card_Write_ApplyLabel,</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>124</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H45" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Read_Labels, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_id","labels"})},</v>
+        <v>{EntityRequestType.Card_Write_ApplyLabel, () =&gt; new Endpoint(RestMethod.Post, new[]{"cards","_id","labels"})},</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2867,28 +2870,28 @@
         <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>175</v>
+        <v>51</v>
       </c>
       <c r="D46" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Read_Members</v>
+        <v>Card_Write_AssignMember</v>
       </c>
       <c r="E46" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Read_Members,</v>
+        <v>Card_Write_AssignMember,</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>190</v>
+        <v>125</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H46" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Read_Members, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_id","members"})},</v>
+        <v>{EntityRequestType.Card_Write_AssignMember, () =&gt; new Endpoint(RestMethod.Post, new[]{"cards","_id","idMembers"})},</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2899,25 +2902,25 @@
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>4</v>
+        <v>188</v>
       </c>
       <c r="D47" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Read_Refresh</v>
+        <v>Card_Read_Attachments</v>
       </c>
       <c r="E47" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Read_Refresh,</v>
+        <v>Card_Read_Attachments,</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H47" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_id"})},</v>
+        <v>{EntityRequestType.Card_Read_Attachments, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_id","attachments"})},</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2928,25 +2931,25 @@
         <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="D48" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Read_VotingMembers</v>
+        <v>Card_Read_CheckItems</v>
       </c>
       <c r="E48" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Read_VotingMembers,</v>
+        <v>Card_Read_CheckItems,</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>215</v>
+        <v>130</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H48" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Read_VotingMembers, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_id","membersVoted"})},</v>
+        <v>{EntityRequestType.Card_Read_CheckItems, () =&gt; new Endpoint(RestMethod.Get, new[]{"checklists","_id","checkItems"})},</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -2954,28 +2957,28 @@
         <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>47</v>
+        <v>381</v>
       </c>
       <c r="D49" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_AddAttachment</v>
+        <v>Card_Read_CheckLists</v>
       </c>
       <c r="E49" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_AddAttachment,</v>
+        <v>Card_Read_CheckLists,</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>121</v>
+        <v>189</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H49" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_AddAttachment, () =&gt; new Endpoint(RestMethod.Post, new[]{"cards","_id","attachments"})},</v>
+        <v>{EntityRequestType.Card_Read_CheckLists, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_id","checklists"})},</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2986,25 +2989,25 @@
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D50" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_AddChecklist</v>
+        <v>Card_Write_ClearNotifications</v>
       </c>
       <c r="E50" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_AddChecklist,</v>
+        <v>Card_Write_ClearNotifications,</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>170</v>
       </c>
       <c r="H50" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_AddChecklist, () =&gt; new Endpoint(RestMethod.Post, new[]{"checklists"})},</v>
+        <v>{EntityRequestType.Card_Write_ClearNotifications, () =&gt; new Endpoint(RestMethod.Post, new[]{"cards","_id","markAssociatedNotificationsRead"})},</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -3015,25 +3018,25 @@
         <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D51" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_AddComment</v>
+        <v>Card_Write_Delete</v>
       </c>
       <c r="E51" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_AddComment,</v>
+        <v>Card_Write_Delete,</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>170</v>
+        <v>17</v>
       </c>
       <c r="H51" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_AddComment, () =&gt; new Endpoint(RestMethod.Post, new[]{"cards","_id","actions","comments"})},</v>
+        <v>{EntityRequestType.Card_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"cards","_id"})},</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -3044,25 +3047,25 @@
         <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="D52" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_ApplyLabel</v>
+        <v>Card_Write_Description</v>
       </c>
       <c r="E52" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_ApplyLabel,</v>
+        <v>Card_Write_Description,</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H52" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_ApplyLabel, () =&gt; new Endpoint(RestMethod.Post, new[]{"cards","_id","labels"})},</v>
+        <v>{EntityRequestType.Card_Write_Description, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_id"})},</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -3073,25 +3076,25 @@
         <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D53" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_AssignMember</v>
+        <v>Card_Write_DueDate</v>
       </c>
       <c r="E53" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_AssignMember,</v>
+        <v>Card_Write_DueDate,</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H53" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_AssignMember, () =&gt; new Endpoint(RestMethod.Post, new[]{"cards","_id","idMembers"})},</v>
+        <v>{EntityRequestType.Card_Write_DueDate, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_id"})},</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -3102,25 +3105,25 @@
         <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="D54" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_ClearNotifications</v>
+        <v>Card_Write_IsClosed</v>
       </c>
       <c r="E54" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_ClearNotifications,</v>
+        <v>Card_Write_IsClosed,</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H54" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_ClearNotifications, () =&gt; new Endpoint(RestMethod.Post, new[]{"cards","_id","markAssociatedNotificationsRead"})},</v>
+        <v>{EntityRequestType.Card_Write_IsClosed, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_id"})},</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -3131,25 +3134,25 @@
         <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D55" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_Delete</v>
+        <v>Card_Write_IsSubscribed</v>
       </c>
       <c r="E55" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_Delete,</v>
+        <v>Card_Write_IsSubscribed,</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>122</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="H55" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"cards","_id"})},</v>
+        <v>{EntityRequestType.Card_Write_IsSubscribed, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_id"})},</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -3157,28 +3160,28 @@
         <v>43</v>
       </c>
       <c r="B56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
+        <v>213</v>
       </c>
       <c r="D56" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_Description</v>
+        <v>Card_Read_Labels</v>
       </c>
       <c r="E56" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_Description,</v>
+        <v>Card_Read_Labels,</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H56" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_Description, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_id"})},</v>
+        <v>{EntityRequestType.Card_Read_Labels, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_id","labels"})},</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -3186,28 +3189,28 @@
         <v>43</v>
       </c>
       <c r="B57" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C57" t="s">
-        <v>44</v>
+        <v>175</v>
       </c>
       <c r="D57" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_DueDate</v>
+        <v>Card_Read_Members</v>
       </c>
       <c r="E57" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_DueDate,</v>
+        <v>Card_Read_Members,</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>122</v>
+        <v>190</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H57" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_DueDate, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_id"})},</v>
+        <v>{EntityRequestType.Card_Read_Members, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_id","members"})},</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -3218,15 +3221,15 @@
         <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="D58" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_IsClosed</v>
+        <v>Card_Write_Move</v>
       </c>
       <c r="E58" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_IsClosed,</v>
+        <v>Card_Write_Move,</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>122</v>
@@ -3236,7 +3239,7 @@
       </c>
       <c r="H58" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_IsClosed, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_id"})},</v>
+        <v>{EntityRequestType.Card_Write_Move, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_id"})},</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -3247,15 +3250,15 @@
         <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D59" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_IsSubscribed</v>
+        <v>Card_Write_Name</v>
       </c>
       <c r="E59" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_IsSubscribed,</v>
+        <v>Card_Write_Name,</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>122</v>
@@ -3265,7 +3268,7 @@
       </c>
       <c r="H59" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_IsSubscribed, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_id"})},</v>
+        <v>{EntityRequestType.Card_Write_Name, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_id"})},</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -3276,15 +3279,15 @@
         <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D60" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_Move</v>
+        <v>Card_Write_Position</v>
       </c>
       <c r="E60" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_Move,</v>
+        <v>Card_Write_Position,</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>122</v>
@@ -3294,7 +3297,7 @@
       </c>
       <c r="H60" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_Move, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_id"})},</v>
+        <v>{EntityRequestType.Card_Write_Position, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_id"})},</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3302,28 +3305,28 @@
         <v>43</v>
       </c>
       <c r="B61" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C61" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D61" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_Name</v>
+        <v>Card_Read_Refresh</v>
       </c>
       <c r="E61" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_Name,</v>
+        <v>Card_Read_Refresh,</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>122</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H61" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_Name, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_id"})},</v>
+        <v>{EntityRequestType.Card_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_id"})},</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3334,25 +3337,25 @@
         <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D62" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_Position</v>
+        <v>Card_Write_RemoveLabel</v>
       </c>
       <c r="E62" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_Position,</v>
+        <v>Card_Write_RemoveLabel,</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>171</v>
+        <v>17</v>
       </c>
       <c r="H62" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_Position, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_id"})},</v>
+        <v>{EntityRequestType.Card_Write_RemoveLabel, () =&gt; new Endpoint(RestMethod.Delete, new[]{"cards","_id","labels","_color"})},</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -3363,25 +3366,25 @@
         <v>12</v>
       </c>
       <c r="C63" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="D63" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_RemoveLabel</v>
+        <v>Card_Write_RemoveMember</v>
       </c>
       <c r="E63" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_RemoveLabel,</v>
+        <v>Card_Write_RemoveMember,</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H63" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_RemoveLabel, () =&gt; new Endpoint(RestMethod.Delete, new[]{"cards","_id","labels","_color"})},</v>
+        <v>{EntityRequestType.Card_Write_RemoveMember, () =&gt; new Endpoint(RestMethod.Delete, new[]{"cards","_id","members","_memberId"})},</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -3389,28 +3392,28 @@
         <v>43</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C64" t="s">
-        <v>23</v>
+        <v>214</v>
       </c>
       <c r="D64" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Card_Write_RemoveMember</v>
+        <v>Card_Read_VotingMembers</v>
       </c>
       <c r="E64" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Card_Write_RemoveMember,</v>
+        <v>Card_Read_VotingMembers,</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>128</v>
+        <v>215</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>17</v>
+        <v>168</v>
       </c>
       <c r="H64" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Card_Write_RemoveMember, () =&gt; new Endpoint(RestMethod.Delete, new[]{"cards","_id","members","_memberId"})},</v>
+        <v>{EntityRequestType.Card_Read_VotingMembers, () =&gt; new Endpoint(RestMethod.Get, new[]{"cards","_id","membersVoted"})},</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -3447,28 +3450,28 @@
         <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C66" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D66" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>CheckItem_Read_Refresh</v>
+        <v>CheckItem_Write_Delete</v>
       </c>
       <c r="E66" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>CheckItem_Read_Refresh,</v>
+        <v>CheckItem_Write_Delete,</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>129</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>168</v>
+        <v>17</v>
       </c>
       <c r="H66" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.CheckItem_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"checklists","_checkListId","checkItems","_id"})},</v>
+        <v>{EntityRequestType.CheckItem_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"checklists","_checkListId","checkItems","_id"})},</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -3479,25 +3482,25 @@
         <v>12</v>
       </c>
       <c r="C67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D67" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>CheckItem_Write_Delete</v>
+        <v>CheckItem_Write_Name</v>
       </c>
       <c r="E67" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>CheckItem_Write_Delete,</v>
+        <v>CheckItem_Write_Name,</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>129</v>
+        <v>218</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="H67" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.CheckItem_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"checklists","_checkListId","checkItems","_id"})},</v>
+        <v>{EntityRequestType.CheckItem_Write_Name, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_cardId","checklist","_checkListId","checkItem","_id","name"})},</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -3508,25 +3511,25 @@
         <v>12</v>
       </c>
       <c r="C68" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D68" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>CheckItem_Write_Name</v>
+        <v>CheckItem_Write_Position</v>
       </c>
       <c r="E68" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>CheckItem_Write_Name,</v>
+        <v>CheckItem_Write_Position,</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>171</v>
       </c>
       <c r="H68" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.CheckItem_Write_Name, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_cardId","checklist","_checkListId","checkItem","_id","name"})},</v>
+        <v>{EntityRequestType.CheckItem_Write_Position, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_cardId","checklist","_checkListId","checkItem","_id","pos"})},</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -3534,28 +3537,28 @@
         <v>55</v>
       </c>
       <c r="B69" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C69" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="D69" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>CheckItem_Write_Position</v>
+        <v>CheckItem_Read_Refresh</v>
       </c>
       <c r="E69" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>CheckItem_Write_Position,</v>
+        <v>CheckItem_Read_Refresh,</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>219</v>
+        <v>129</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H69" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.CheckItem_Write_Position, () =&gt; new Endpoint(RestMethod.Put, new[]{"cards","_cardId","checklist","_checkListId","checkItem","_id","pos"})},</v>
+        <v>{EntityRequestType.CheckItem_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"checklists","_checkListId","checkItems","_id"})},</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -3592,28 +3595,28 @@
         <v>57</v>
       </c>
       <c r="B71" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>191</v>
+        <v>58</v>
       </c>
       <c r="D71" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>CheckList_Read_CheckItems</v>
+        <v>CheckList_Write_AddCheckItem</v>
       </c>
       <c r="E71" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>CheckList_Read_CheckItems,</v>
+        <v>CheckList_Write_AddCheckItem,</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>130</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H71" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.CheckList_Read_CheckItems, () =&gt; new Endpoint(RestMethod.Get, new[]{"checklists","_id","checkItems"})},</v>
+        <v>{EntityRequestType.CheckList_Write_AddCheckItem, () =&gt; new Endpoint(RestMethod.Post, new[]{"checklists","_id","checkItems"})},</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -3621,28 +3624,28 @@
         <v>57</v>
       </c>
       <c r="B72" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C72" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="D72" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>CheckList_Read_Refresh</v>
+        <v>CheckList_Write_Card</v>
       </c>
       <c r="E72" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>CheckList_Read_Refresh,</v>
+        <v>CheckList_Write_Card,</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>131</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H72" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.CheckList_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"checklists","_id"})},</v>
+        <v>{EntityRequestType.CheckList_Write_Card, () =&gt; new Endpoint(RestMethod.Put, new[]{"checklists","_id"})},</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -3650,28 +3653,28 @@
         <v>57</v>
       </c>
       <c r="B73" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C73" t="s">
-        <v>58</v>
+        <v>191</v>
       </c>
       <c r="D73" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>CheckList_Write_AddCheckItem</v>
+        <v>CheckList_Read_CheckItems</v>
       </c>
       <c r="E73" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>CheckList_Write_AddCheckItem,</v>
+        <v>CheckList_Read_CheckItems,</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>130</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H73" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.CheckList_Write_AddCheckItem, () =&gt; new Endpoint(RestMethod.Post, new[]{"checklists","_id","checkItems"})},</v>
+        <v>{EntityRequestType.CheckList_Read_CheckItems, () =&gt; new Endpoint(RestMethod.Get, new[]{"checklists","_id","checkItems"})},</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -3682,25 +3685,25 @@
         <v>12</v>
       </c>
       <c r="C74" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="D74" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>CheckList_Write_Card</v>
+        <v>CheckList_Write_Delete</v>
       </c>
       <c r="E74" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>CheckList_Write_Card,</v>
+        <v>CheckList_Write_Delete,</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>131</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>171</v>
+        <v>17</v>
       </c>
       <c r="H74" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.CheckList_Write_Card, () =&gt; new Endpoint(RestMethod.Put, new[]{"checklists","_id"})},</v>
+        <v>{EntityRequestType.CheckList_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"checklists","_id"})},</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3711,25 +3714,25 @@
         <v>12</v>
       </c>
       <c r="C75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D75" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>CheckList_Write_Delete</v>
+        <v>CheckList_Write_Name</v>
       </c>
       <c r="E75" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>CheckList_Write_Delete,</v>
+        <v>CheckList_Write_Name,</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>131</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="H75" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.CheckList_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"checklists","_id"})},</v>
+        <v>{EntityRequestType.CheckList_Write_Name, () =&gt; new Endpoint(RestMethod.Put, new[]{"checklists","_id"})},</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -3740,15 +3743,15 @@
         <v>12</v>
       </c>
       <c r="C76" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D76" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>CheckList_Write_Name</v>
+        <v>CheckList_Write_Position</v>
       </c>
       <c r="E76" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>CheckList_Write_Name,</v>
+        <v>CheckList_Write_Position,</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>131</v>
@@ -3758,7 +3761,7 @@
       </c>
       <c r="H76" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.CheckList_Write_Name, () =&gt; new Endpoint(RestMethod.Put, new[]{"checklists","_id"})},</v>
+        <v>{EntityRequestType.CheckList_Write_Position, () =&gt; new Endpoint(RestMethod.Put, new[]{"checklists","_id"})},</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3766,28 +3769,28 @@
         <v>57</v>
       </c>
       <c r="B77" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C77" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="D77" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>CheckList_Write_Position</v>
+        <v>CheckList_Read_Refresh</v>
       </c>
       <c r="E77" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>CheckList_Write_Position,</v>
+        <v>CheckList_Read_Refresh,</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>131</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H77" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.CheckList_Write_Position, () =&gt; new Endpoint(RestMethod.Put, new[]{"checklists","_id"})},</v>
+        <v>{EntityRequestType.CheckList_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"checklists","_id"})},</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3824,28 +3827,28 @@
         <v>132</v>
       </c>
       <c r="B79" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C79" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="D79" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>LabelNames_Read_Refresh</v>
+        <v>LabelNames_Write_Blue</v>
       </c>
       <c r="E79" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>LabelNames_Read_Refresh,</v>
+        <v>LabelNames_Write_Blue,</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H79" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.LabelNames_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"board","_boardId","labelNames"})},</v>
+        <v>{EntityRequestType.LabelNames_Write_Blue, () =&gt; new Endpoint(RestMethod.Put, new[]{"board","_boardId","labelNames","_color"})},</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3856,15 +3859,15 @@
         <v>12</v>
       </c>
       <c r="C80" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D80" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>LabelNames_Write_Blue</v>
+        <v>LabelNames_Write_Green</v>
       </c>
       <c r="E80" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>LabelNames_Write_Blue,</v>
+        <v>LabelNames_Write_Green,</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>133</v>
@@ -3874,7 +3877,7 @@
       </c>
       <c r="H80" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.LabelNames_Write_Blue, () =&gt; new Endpoint(RestMethod.Put, new[]{"board","_boardId","labelNames","_color"})},</v>
+        <v>{EntityRequestType.LabelNames_Write_Green, () =&gt; new Endpoint(RestMethod.Put, new[]{"board","_boardId","labelNames","_color"})},</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -3885,15 +3888,15 @@
         <v>12</v>
       </c>
       <c r="C81" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D81" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>LabelNames_Write_Green</v>
+        <v>LabelNames_Write_Orange</v>
       </c>
       <c r="E81" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>LabelNames_Write_Green,</v>
+        <v>LabelNames_Write_Orange,</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>133</v>
@@ -3903,7 +3906,7 @@
       </c>
       <c r="H81" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.LabelNames_Write_Green, () =&gt; new Endpoint(RestMethod.Put, new[]{"board","_boardId","labelNames","_color"})},</v>
+        <v>{EntityRequestType.LabelNames_Write_Orange, () =&gt; new Endpoint(RestMethod.Put, new[]{"board","_boardId","labelNames","_color"})},</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -3914,15 +3917,15 @@
         <v>12</v>
       </c>
       <c r="C82" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D82" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>LabelNames_Write_Orange</v>
+        <v>LabelNames_Write_Purple</v>
       </c>
       <c r="E82" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>LabelNames_Write_Orange,</v>
+        <v>LabelNames_Write_Purple,</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>133</v>
@@ -3932,7 +3935,7 @@
       </c>
       <c r="H82" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.LabelNames_Write_Orange, () =&gt; new Endpoint(RestMethod.Put, new[]{"board","_boardId","labelNames","_color"})},</v>
+        <v>{EntityRequestType.LabelNames_Write_Purple, () =&gt; new Endpoint(RestMethod.Put, new[]{"board","_boardId","labelNames","_color"})},</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -3943,15 +3946,15 @@
         <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D83" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>LabelNames_Write_Purple</v>
+        <v>LabelNames_Write_Red</v>
       </c>
       <c r="E83" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>LabelNames_Write_Purple,</v>
+        <v>LabelNames_Write_Red,</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>133</v>
@@ -3961,7 +3964,7 @@
       </c>
       <c r="H83" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.LabelNames_Write_Purple, () =&gt; new Endpoint(RestMethod.Put, new[]{"board","_boardId","labelNames","_color"})},</v>
+        <v>{EntityRequestType.LabelNames_Write_Red, () =&gt; new Endpoint(RestMethod.Put, new[]{"board","_boardId","labelNames","_color"})},</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -3969,28 +3972,28 @@
         <v>132</v>
       </c>
       <c r="B84" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C84" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="D84" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>LabelNames_Write_Red</v>
+        <v>LabelNames_Read_Refresh</v>
       </c>
       <c r="E84" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>LabelNames_Write_Red,</v>
+        <v>LabelNames_Read_Refresh,</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H84" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.LabelNames_Write_Red, () =&gt; new Endpoint(RestMethod.Put, new[]{"board","_boardId","labelNames","_color"})},</v>
+        <v>{EntityRequestType.LabelNames_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"board","_boardId","labelNames"})},</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -4056,28 +4059,28 @@
         <v>66</v>
       </c>
       <c r="B87" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C87" t="s">
-        <v>174</v>
+        <v>67</v>
       </c>
       <c r="D87" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>List_Read_Cards</v>
+        <v>List_Write_AddCard</v>
       </c>
       <c r="E87" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>List_Read_Cards,</v>
+        <v>List_Write_AddCard,</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>193</v>
+        <v>134</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H87" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.List_Read_Cards, () =&gt; new Endpoint(RestMethod.Get, new[]{"lists","_id","cards"})},</v>
+        <v>{EntityRequestType.List_Write_AddCard, () =&gt; new Endpoint(RestMethod.Post, new[]{"cards"})},</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -4085,28 +4088,28 @@
         <v>66</v>
       </c>
       <c r="B88" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D88" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>List_Read_Refresh</v>
+        <v>List_Write_Board</v>
       </c>
       <c r="E88" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>List_Read_Refresh,</v>
+        <v>List_Write_Board,</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>136</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H88" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.List_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"lists","_id"})},</v>
+        <v>{EntityRequestType.List_Write_Board, () =&gt; new Endpoint(RestMethod.Put, new[]{"lists","_id"})},</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -4114,28 +4117,28 @@
         <v>66</v>
       </c>
       <c r="B89" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C89" t="s">
-        <v>67</v>
+        <v>174</v>
       </c>
       <c r="D89" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>List_Write_AddCard</v>
+        <v>List_Read_Cards</v>
       </c>
       <c r="E89" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>List_Write_AddCard,</v>
+        <v>List_Read_Cards,</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>134</v>
+        <v>193</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H89" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.List_Write_AddCard, () =&gt; new Endpoint(RestMethod.Post, new[]{"cards"})},</v>
+        <v>{EntityRequestType.List_Read_Cards, () =&gt; new Endpoint(RestMethod.Get, new[]{"lists","_id","cards"})},</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -4146,25 +4149,25 @@
         <v>12</v>
       </c>
       <c r="C90" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D90" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>List_Write_Board</v>
+        <v>List_Write_Delete</v>
       </c>
       <c r="E90" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>List_Write_Board,</v>
+        <v>List_Write_Delete,</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>136</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>171</v>
+        <v>17</v>
       </c>
       <c r="H90" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.List_Write_Board, () =&gt; new Endpoint(RestMethod.Put, new[]{"lists","_id"})},</v>
+        <v>{EntityRequestType.List_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"lists","_id"})},</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -4175,25 +4178,25 @@
         <v>12</v>
       </c>
       <c r="C91" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D91" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>List_Write_Delete</v>
+        <v>List_Write_IsClosed</v>
       </c>
       <c r="E91" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>List_Write_Delete,</v>
+        <v>List_Write_IsClosed,</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>136</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="H91" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.List_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"lists","_id"})},</v>
+        <v>{EntityRequestType.List_Write_IsClosed, () =&gt; new Endpoint(RestMethod.Put, new[]{"lists","_id"})},</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -4204,15 +4207,15 @@
         <v>12</v>
       </c>
       <c r="C92" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D92" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>List_Write_IsClosed</v>
+        <v>List_Write_IsSubscribed</v>
       </c>
       <c r="E92" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>List_Write_IsClosed,</v>
+        <v>List_Write_IsSubscribed,</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>136</v>
@@ -4222,7 +4225,7 @@
       </c>
       <c r="H92" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.List_Write_IsClosed, () =&gt; new Endpoint(RestMethod.Put, new[]{"lists","_id"})},</v>
+        <v>{EntityRequestType.List_Write_IsSubscribed, () =&gt; new Endpoint(RestMethod.Put, new[]{"lists","_id"})},</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -4233,15 +4236,15 @@
         <v>12</v>
       </c>
       <c r="C93" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="D93" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>List_Write_IsSubscribed</v>
+        <v>List_Write_Move</v>
       </c>
       <c r="E93" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>List_Write_IsSubscribed,</v>
+        <v>List_Write_Move,</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>136</v>
@@ -4251,7 +4254,7 @@
       </c>
       <c r="H93" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.List_Write_IsSubscribed, () =&gt; new Endpoint(RestMethod.Put, new[]{"lists","_id"})},</v>
+        <v>{EntityRequestType.List_Write_Move, () =&gt; new Endpoint(RestMethod.Put, new[]{"lists","_id"})},</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -4262,15 +4265,15 @@
         <v>12</v>
       </c>
       <c r="C94" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D94" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>List_Write_Move</v>
+        <v>List_Write_Name</v>
       </c>
       <c r="E94" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>List_Write_Move,</v>
+        <v>List_Write_Name,</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>136</v>
@@ -4280,7 +4283,7 @@
       </c>
       <c r="H94" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.List_Write_Move, () =&gt; new Endpoint(RestMethod.Put, new[]{"lists","_id"})},</v>
+        <v>{EntityRequestType.List_Write_Name, () =&gt; new Endpoint(RestMethod.Put, new[]{"lists","_id"})},</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -4291,15 +4294,15 @@
         <v>12</v>
       </c>
       <c r="C95" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D95" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>List_Write_Name</v>
+        <v>List_Write_Position</v>
       </c>
       <c r="E95" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>List_Write_Name,</v>
+        <v>List_Write_Position,</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>136</v>
@@ -4309,7 +4312,7 @@
       </c>
       <c r="H95" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.List_Write_Name, () =&gt; new Endpoint(RestMethod.Put, new[]{"lists","_id"})},</v>
+        <v>{EntityRequestType.List_Write_Position, () =&gt; new Endpoint(RestMethod.Put, new[]{"lists","_id"})},</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -4317,28 +4320,28 @@
         <v>66</v>
       </c>
       <c r="B96" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C96" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="D96" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>List_Write_Position</v>
+        <v>List_Read_Refresh</v>
       </c>
       <c r="E96" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>List_Write_Position,</v>
+        <v>List_Read_Refresh,</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>136</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H96" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.List_Write_Position, () =&gt; new Endpoint(RestMethod.Put, new[]{"lists","_id"})},</v>
+        <v>{EntityRequestType.List_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"lists","_id"})},</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -4375,28 +4378,28 @@
         <v>6</v>
       </c>
       <c r="B98" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C98" t="s">
-        <v>195</v>
+        <v>68</v>
       </c>
       <c r="D98" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Read_Boards</v>
+        <v>Member_Write_AvatarSource</v>
       </c>
       <c r="E98" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Read_Boards,</v>
+        <v>Member_Write_AvatarSource,</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>212</v>
+        <v>137</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H98" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Read_Boards, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","boards"})},</v>
+        <v>{EntityRequestType.Member_Write_AvatarSource, () =&gt; new Endpoint(RestMethod.Put, new[]{"members","_id"})},</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -4404,28 +4407,28 @@
         <v>6</v>
       </c>
       <c r="B99" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C99" t="s">
-        <v>174</v>
+        <v>69</v>
       </c>
       <c r="D99" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Read_Cards</v>
+        <v>Member_Write_Bio</v>
       </c>
       <c r="E99" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Read_Cards,</v>
+        <v>Member_Write_Bio,</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>196</v>
+        <v>137</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H99" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Read_Cards, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","cards"})},</v>
+        <v>{EntityRequestType.Member_Write_Bio, () =&gt; new Endpoint(RestMethod.Put, new[]{"members","_id"})},</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -4436,25 +4439,25 @@
         <v>11</v>
       </c>
       <c r="C100" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D100" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Read_InvitedBoards</v>
+        <v>Member_Read_Boards</v>
       </c>
       <c r="E100" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Read_InvitedBoards,</v>
+        <v>Member_Read_Boards,</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H100" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Read_InvitedBoards, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","boardsInvited"})},</v>
+        <v>{EntityRequestType.Member_Read_Boards, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","boards"})},</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -4465,25 +4468,25 @@
         <v>11</v>
       </c>
       <c r="C101" t="s">
-        <v>202</v>
+        <v>174</v>
       </c>
       <c r="D101" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Read_InvitedOrganizations</v>
+        <v>Member_Read_Cards</v>
       </c>
       <c r="E101" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Read_InvitedOrganizations,</v>
+        <v>Member_Read_Cards,</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H101" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Read_InvitedOrganizations, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","organizationsInvited"})},</v>
+        <v>{EntityRequestType.Member_Read_Cards, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","cards"})},</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -4491,28 +4494,28 @@
         <v>6</v>
       </c>
       <c r="B102" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C102" t="s">
-        <v>197</v>
+        <v>52</v>
       </c>
       <c r="D102" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Read_Notifications</v>
+        <v>Member_Write_ClearNotifications</v>
       </c>
       <c r="E102" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Read_Notifications,</v>
+        <v>Member_Write_ClearNotifications,</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H102" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Read_Notifications, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","notifications"})},</v>
+        <v>{EntityRequestType.Member_Write_ClearNotifications, () =&gt; new Endpoint(RestMethod.Post, new[]{"notifications","all","read"})},</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -4520,28 +4523,28 @@
         <v>6</v>
       </c>
       <c r="B103" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="D103" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Read_Organization</v>
+        <v>Member_Write_CreateBoard</v>
       </c>
       <c r="E103" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Read_Organization,</v>
+        <v>Member_Write_CreateBoard,</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H103" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Read_Organization, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","organizations"})},</v>
+        <v>{EntityRequestType.Member_Write_CreateBoard, () =&gt; new Endpoint(RestMethod.Post, new[]{"boards"})},</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -4549,28 +4552,28 @@
         <v>6</v>
       </c>
       <c r="B104" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C104" t="s">
-        <v>380</v>
+        <v>236</v>
       </c>
       <c r="D104" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Read_Organizations</v>
+        <v>Member_Write_CreateOrganization</v>
       </c>
       <c r="E104" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Read_Organizations,</v>
+        <v>Member_Write_CreateOrganization,</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>381</v>
+        <v>139</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H104" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Read_Organizations, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","idOrganizations"})},</v>
+        <v>{EntityRequestType.Member_Write_CreateOrganization, () =&gt; new Endpoint(RestMethod.Post, new[]{"organizations"})},</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -4578,28 +4581,28 @@
         <v>6</v>
       </c>
       <c r="B105" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C105" t="s">
-        <v>379</v>
+        <v>70</v>
       </c>
       <c r="D105" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Read_PinnedBoards</v>
+        <v>Member_Write_FullName</v>
       </c>
       <c r="E105" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Read_PinnedBoards,</v>
+        <v>Member_Write_FullName,</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H105" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Read_PinnedBoards, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","idBoardsPinned"})},</v>
+        <v>{EntityRequestType.Member_Write_FullName, () =&gt; new Endpoint(RestMethod.Put, new[]{"members","_id"})},</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -4607,28 +4610,28 @@
         <v>6</v>
       </c>
       <c r="B106" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C106" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="D106" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Read_Refresh</v>
+        <v>Member_Write_Initials</v>
       </c>
       <c r="E106" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Read_Refresh,</v>
+        <v>Member_Write_Initials,</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>137</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H106" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id"})},</v>
+        <v>{EntityRequestType.Member_Write_Initials, () =&gt; new Endpoint(RestMethod.Put, new[]{"members","_id"})},</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -4639,25 +4642,25 @@
         <v>11</v>
       </c>
       <c r="C107" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D107" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Read_Sessions</v>
+        <v>Member_Read_InvitedBoards</v>
       </c>
       <c r="E107" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Read_Sessions,</v>
+        <v>Member_Read_InvitedBoards,</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H107" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Read_Sessions, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","sessions"})},</v>
+        <v>{EntityRequestType.Member_Read_InvitedBoards, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","boardsInvited"})},</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -4668,25 +4671,25 @@
         <v>11</v>
       </c>
       <c r="C108" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D108" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Read_Tokens</v>
+        <v>Member_Read_InvitedOrganizations</v>
       </c>
       <c r="E108" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Read_Tokens,</v>
+        <v>Member_Read_InvitedOrganizations,</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H108" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Read_Tokens, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","tokens"})},</v>
+        <v>{EntityRequestType.Member_Read_InvitedOrganizations, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","organizationsInvited"})},</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -4694,28 +4697,28 @@
         <v>6</v>
       </c>
       <c r="B109" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C109" t="s">
-        <v>68</v>
+        <v>197</v>
       </c>
       <c r="D109" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Write_AvatarSource</v>
+        <v>Member_Read_Notifications</v>
       </c>
       <c r="E109" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Write_AvatarSource,</v>
+        <v>Member_Read_Notifications,</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>137</v>
+        <v>198</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H109" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Write_AvatarSource, () =&gt; new Endpoint(RestMethod.Put, new[]{"members","_id"})},</v>
+        <v>{EntityRequestType.Member_Read_Notifications, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","notifications"})},</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -4723,28 +4726,28 @@
         <v>6</v>
       </c>
       <c r="B110" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C110" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="D110" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Write_Bio</v>
+        <v>Member_Read_Organization</v>
       </c>
       <c r="E110" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Write_Bio,</v>
+        <v>Member_Read_Organization,</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>137</v>
+        <v>199</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H110" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Write_Bio, () =&gt; new Endpoint(RestMethod.Put, new[]{"members","_id"})},</v>
+        <v>{EntityRequestType.Member_Read_Organization, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","organizations"})},</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -4752,28 +4755,28 @@
         <v>6</v>
       </c>
       <c r="B111" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C111" t="s">
-        <v>52</v>
+        <v>379</v>
       </c>
       <c r="D111" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Write_ClearNotifications</v>
+        <v>Member_Read_Organizations</v>
       </c>
       <c r="E111" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Write_ClearNotifications,</v>
+        <v>Member_Read_Organizations,</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>172</v>
+        <v>380</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H111" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Write_ClearNotifications, () =&gt; new Endpoint(RestMethod.Post, new[]{"notifications","all","read"})},</v>
+        <v>{EntityRequestType.Member_Read_Organizations, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","idOrganizations"})},</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -4784,25 +4787,25 @@
         <v>12</v>
       </c>
       <c r="C112" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D112" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Write_CreateBoard</v>
+        <v>Member_Write_PinBoard</v>
       </c>
       <c r="E112" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Write_CreateBoard,</v>
+        <v>Member_Write_PinBoard,</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>170</v>
       </c>
       <c r="H112" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Write_CreateBoard, () =&gt; new Endpoint(RestMethod.Post, new[]{"boards"})},</v>
+        <v>{EntityRequestType.Member_Write_PinBoard, () =&gt; new Endpoint(RestMethod.Post, new[]{"members","_id","idBoardsPinned"})},</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -4810,28 +4813,28 @@
         <v>6</v>
       </c>
       <c r="B113" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C113" t="s">
-        <v>236</v>
+        <v>4</v>
       </c>
       <c r="D113" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Write_CreateOrganization</v>
+        <v>Member_Read_Refresh</v>
       </c>
       <c r="E113" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Write_CreateOrganization,</v>
+        <v>Member_Read_Refresh,</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H113" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Write_CreateOrganization, () =&gt; new Endpoint(RestMethod.Post, new[]{"organizations"})},</v>
+        <v>{EntityRequestType.Member_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id"})},</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -4842,25 +4845,25 @@
         <v>12</v>
       </c>
       <c r="C114" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D114" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Write_FullName</v>
+        <v>Member_Write_RescindVoteForCard</v>
       </c>
       <c r="E114" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Write_FullName,</v>
+        <v>Member_Write_RescindVoteForCard,</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>171</v>
+        <v>17</v>
       </c>
       <c r="H114" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Write_FullName, () =&gt; new Endpoint(RestMethod.Put, new[]{"members","_id"})},</v>
+        <v>{EntityRequestType.Member_Write_RescindVoteForCard, () =&gt; new Endpoint(RestMethod.Delete, new[]{"cards","_cardId","membersVoted","_id"})},</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -4868,28 +4871,28 @@
         <v>6</v>
       </c>
       <c r="B115" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C115" t="s">
-        <v>71</v>
+        <v>204</v>
       </c>
       <c r="D115" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Write_Initials</v>
+        <v>Member_Read_Sessions</v>
       </c>
       <c r="E115" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Write_Initials,</v>
+        <v>Member_Read_Sessions,</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>137</v>
+        <v>205</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H115" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Write_Initials, () =&gt; new Endpoint(RestMethod.Put, new[]{"members","_id"})},</v>
+        <v>{EntityRequestType.Member_Read_Sessions, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","sessions"})},</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -4897,28 +4900,28 @@
         <v>6</v>
       </c>
       <c r="B116" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C116" t="s">
-        <v>74</v>
+        <v>383</v>
       </c>
       <c r="D116" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Write_PinBoard</v>
+        <v>Member_Read_StarredBoards</v>
       </c>
       <c r="E116" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Write_PinBoard,</v>
+        <v>Member_Read_StarredBoards,</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>140</v>
+        <v>384</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H116" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Write_PinBoard, () =&gt; new Endpoint(RestMethod.Post, new[]{"members","_id","idBoardsPinned"})},</v>
+        <v>{EntityRequestType.Member_Read_StarredBoards, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","boardStars"})},</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -4926,28 +4929,28 @@
         <v>6</v>
       </c>
       <c r="B117" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C117" t="s">
-        <v>75</v>
+        <v>206</v>
       </c>
       <c r="D117" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Member_Write_RescindVoteForCard</v>
+        <v>Member_Read_Tokens</v>
       </c>
       <c r="E117" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Member_Write_RescindVoteForCard,</v>
+        <v>Member_Read_Tokens,</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>142</v>
+        <v>207</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>17</v>
+        <v>168</v>
       </c>
       <c r="H117" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Member_Write_RescindVoteForCard, () =&gt; new Endpoint(RestMethod.Delete, new[]{"cards","_cardId","membersVoted","_id"})},</v>
+        <v>{EntityRequestType.Member_Read_Tokens, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_id","tokens"})},</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -5042,28 +5045,28 @@
         <v>78</v>
       </c>
       <c r="B121" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C121" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="D121" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>MemberPreferences_Read_Refresh</v>
+        <v>MemberPreferences_Write_ColorBlind</v>
       </c>
       <c r="E121" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>MemberPreferences_Read_Refresh,</v>
+        <v>MemberPreferences_Write_ColorBlind,</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H121" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.MemberPreferences_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_memberId","prefs"})},</v>
+        <v>{EntityRequestType.MemberPreferences_Write_ColorBlind, () =&gt; new Endpoint(RestMethod.Put, new[]{"members","_memberId","prefs","colorBlind"})},</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5074,25 +5077,25 @@
         <v>12</v>
       </c>
       <c r="C122" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D122" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>MemberPreferences_Write_ColorBlind</v>
+        <v>MemberPreferences_Write_MinutesBeforeDeadlineToNotify</v>
       </c>
       <c r="E122" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>MemberPreferences_Write_ColorBlind,</v>
+        <v>MemberPreferences_Write_MinutesBeforeDeadlineToNotify,</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>171</v>
       </c>
       <c r="H122" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.MemberPreferences_Write_ColorBlind, () =&gt; new Endpoint(RestMethod.Put, new[]{"members","_memberId","prefs","colorBlind"})},</v>
+        <v>{EntityRequestType.MemberPreferences_Write_MinutesBeforeDeadlineToNotify, () =&gt; new Endpoint(RestMethod.Put, new[]{"members","_memberId","prefs","minutesBeforeDeadlineToNotify"})},</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5103,25 +5106,25 @@
         <v>12</v>
       </c>
       <c r="C123" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D123" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>MemberPreferences_Write_MinutesBeforeDeadlineToNotify</v>
+        <v>MemberPreferences_Write_MinutesBetweenSummaries</v>
       </c>
       <c r="E123" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>MemberPreferences_Write_MinutesBeforeDeadlineToNotify,</v>
+        <v>MemberPreferences_Write_MinutesBetweenSummaries,</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>171</v>
       </c>
       <c r="H123" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.MemberPreferences_Write_MinutesBeforeDeadlineToNotify, () =&gt; new Endpoint(RestMethod.Put, new[]{"members","_memberId","prefs","minutesBeforeDeadlineToNotify"})},</v>
+        <v>{EntityRequestType.MemberPreferences_Write_MinutesBetweenSummaries, () =&gt; new Endpoint(RestMethod.Put, new[]{"members","_memberId","prefs","minutesBetweenSummaries"})},</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -5129,28 +5132,28 @@
         <v>78</v>
       </c>
       <c r="B124" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C124" t="s">
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D124" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>MemberPreferences_Write_MinutesBetweenSummaries</v>
+        <v>MemberPreferences_Read_Refresh</v>
       </c>
       <c r="E124" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>MemberPreferences_Write_MinutesBetweenSummaries,</v>
+        <v>MemberPreferences_Read_Refresh,</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H124" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.MemberPreferences_Write_MinutesBetweenSummaries, () =&gt; new Endpoint(RestMethod.Put, new[]{"members","_memberId","prefs","minutesBetweenSummaries"})},</v>
+        <v>{EntityRequestType.MemberPreferences_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"members","_memberId","prefs"})},</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -5216,28 +5219,28 @@
         <v>84</v>
       </c>
       <c r="B127" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C127" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="D127" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Notification_Read_Refresh</v>
+        <v>Notification_Write_IsUnread</v>
       </c>
       <c r="E127" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Notification_Read_Refresh,</v>
+        <v>Notification_Write_IsUnread,</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H127" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Notification_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"notifications","_id"})},</v>
+        <v>{EntityRequestType.Notification_Write_IsUnread, () =&gt; new Endpoint(RestMethod.Put, new[]{"notifications","_id","unread"})},</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -5245,28 +5248,28 @@
         <v>84</v>
       </c>
       <c r="B128" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C128" t="s">
-        <v>85</v>
+        <v>4</v>
       </c>
       <c r="D128" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Notification_Write_IsUnread</v>
+        <v>Notification_Read_Refresh</v>
       </c>
       <c r="E128" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Notification_Write_IsUnread,</v>
+        <v>Notification_Read_Refresh,</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H128" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Notification_Write_IsUnread, () =&gt; new Endpoint(RestMethod.Put, new[]{"notifications","_id","unread"})},</v>
+        <v>{EntityRequestType.Notification_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"notifications","_id"})},</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -5303,28 +5306,28 @@
         <v>18</v>
       </c>
       <c r="B130" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C130" t="s">
-        <v>195</v>
+        <v>20</v>
       </c>
       <c r="D130" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Organization_Read_Boards</v>
+        <v>Organization_Write_AddOrUpdateMember</v>
       </c>
       <c r="E130" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Organization_Read_Boards,</v>
+        <v>Organization_Write_AddOrUpdateMember,</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>209</v>
+        <v>148</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H130" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Organization_Read_Boards, () =&gt; new Endpoint(RestMethod.Get, new[]{"organizations","_id","boards"})},</v>
+        <v>{EntityRequestType.Organization_Write_AddOrUpdateMember, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_id","members","_memberId"})},</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -5335,25 +5338,25 @@
         <v>11</v>
       </c>
       <c r="C131" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="D131" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Organization_Read_InvitedMembers</v>
+        <v>Organization_Read_Boards</v>
       </c>
       <c r="E131" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Organization_Read_InvitedMembers,</v>
+        <v>Organization_Read_Boards,</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G131" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H131" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Organization_Read_InvitedMembers, () =&gt; new Endpoint(RestMethod.Get, new[]{"organizations","_id","membersInvited"})},</v>
+        <v>{EntityRequestType.Organization_Read_Boards, () =&gt; new Endpoint(RestMethod.Get, new[]{"organizations","_id","boards"})},</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -5361,28 +5364,28 @@
         <v>18</v>
       </c>
       <c r="B132" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C132" t="s">
-        <v>175</v>
+        <v>73</v>
       </c>
       <c r="D132" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Organization_Read_Members</v>
+        <v>Organization_Write_CreateBoard</v>
       </c>
       <c r="E132" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Organization_Read_Members,</v>
+        <v>Organization_Write_CreateBoard,</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H132" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Organization_Read_Members, () =&gt; new Endpoint(RestMethod.Get, new[]{"organizations","_id","members"})},</v>
+        <v>{EntityRequestType.Organization_Write_CreateBoard, () =&gt; new Endpoint(RestMethod.Post, new[]{"boards"})},</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -5390,28 +5393,28 @@
         <v>18</v>
       </c>
       <c r="B133" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C133" t="s">
-        <v>176</v>
+        <v>17</v>
       </c>
       <c r="D133" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Organization_Read_Memberships</v>
+        <v>Organization_Write_Delete</v>
       </c>
       <c r="E133" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Organization_Read_Memberships,</v>
+        <v>Organization_Write_Delete,</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>211</v>
+        <v>147</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>168</v>
+        <v>17</v>
       </c>
       <c r="H133" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Organization_Read_Memberships, () =&gt; new Endpoint(RestMethod.Get, new[]{"organizations","_id","memberships"})},</v>
+        <v>{EntityRequestType.Organization_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"organizations","_id"})},</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -5419,28 +5422,28 @@
         <v>18</v>
       </c>
       <c r="B134" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C134" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D134" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Organization_Read_Refresh</v>
+        <v>Organization_Write_Description</v>
       </c>
       <c r="E134" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Organization_Read_Refresh,</v>
+        <v>Organization_Write_Description,</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>147</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H134" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Organization_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"organizations","_id"})},</v>
+        <v>{EntityRequestType.Organization_Write_Description, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_id"})},</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -5451,25 +5454,25 @@
         <v>12</v>
       </c>
       <c r="C135" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="D135" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Organization_Write_AddOrUpdateMember</v>
+        <v>Organization_Write_DisplayName</v>
       </c>
       <c r="E135" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Organization_Write_AddOrUpdateMember,</v>
+        <v>Organization_Write_DisplayName,</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G135" s="1" t="s">
         <v>171</v>
       </c>
       <c r="H135" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Organization_Write_AddOrUpdateMember, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_id","members","_memberId"})},</v>
+        <v>{EntityRequestType.Organization_Write_DisplayName, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_id"})},</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -5477,28 +5480,28 @@
         <v>18</v>
       </c>
       <c r="B136" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C136" t="s">
-        <v>73</v>
+        <v>177</v>
       </c>
       <c r="D136" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Organization_Write_CreateBoard</v>
+        <v>Organization_Read_InvitedMembers</v>
       </c>
       <c r="E136" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Organization_Write_CreateBoard,</v>
+        <v>Organization_Read_InvitedMembers,</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>138</v>
+        <v>210</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H136" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Organization_Write_CreateBoard, () =&gt; new Endpoint(RestMethod.Post, new[]{"boards"})},</v>
+        <v>{EntityRequestType.Organization_Read_InvitedMembers, () =&gt; new Endpoint(RestMethod.Get, new[]{"organizations","_id","membersInvited"})},</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -5509,25 +5512,25 @@
         <v>12</v>
       </c>
       <c r="C137" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D137" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Organization_Write_Delete</v>
+        <v>Organization_Write_InviteMember</v>
       </c>
       <c r="E137" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Organization_Write_Delete,</v>
+        <v>Organization_Write_InviteMember,</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>17</v>
+        <v>170</v>
       </c>
       <c r="H137" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Organization_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"organizations","_id"})},</v>
+        <v>{EntityRequestType.Organization_Write_InviteMember, () =&gt; new Endpoint(RestMethod.Post, new[]{string.Empty})},</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -5535,28 +5538,28 @@
         <v>18</v>
       </c>
       <c r="B138" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C138" t="s">
-        <v>9</v>
+        <v>175</v>
       </c>
       <c r="D138" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Organization_Write_Description</v>
+        <v>Organization_Read_Members</v>
       </c>
       <c r="E138" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Organization_Write_Description,</v>
+        <v>Organization_Read_Members,</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H138" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Organization_Write_Description, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_id"})},</v>
+        <v>{EntityRequestType.Organization_Read_Members, () =&gt; new Endpoint(RestMethod.Get, new[]{"organizations","_id","members"})},</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -5564,28 +5567,28 @@
         <v>18</v>
       </c>
       <c r="B139" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C139" t="s">
-        <v>86</v>
+        <v>176</v>
       </c>
       <c r="D139" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Organization_Write_DisplayName</v>
+        <v>Organization_Read_Memberships</v>
       </c>
       <c r="E139" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Organization_Write_DisplayName,</v>
+        <v>Organization_Read_Memberships,</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>147</v>
+        <v>211</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H139" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Organization_Write_DisplayName, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_id"})},</v>
+        <v>{EntityRequestType.Organization_Read_Memberships, () =&gt; new Endpoint(RestMethod.Get, new[]{"organizations","_id","memberships"})},</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -5596,25 +5599,25 @@
         <v>12</v>
       </c>
       <c r="C140" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D140" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Organization_Write_InviteMember</v>
+        <v>Organization_Write_Name</v>
       </c>
       <c r="E140" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Organization_Write_InviteMember,</v>
+        <v>Organization_Write_Name,</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H140" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Organization_Write_InviteMember, () =&gt; new Endpoint(RestMethod.Post, new[]{string.Empty})},</v>
+        <v>{EntityRequestType.Organization_Write_Name, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_id"})},</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -5622,28 +5625,28 @@
         <v>18</v>
       </c>
       <c r="B141" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C141" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D141" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Organization_Write_Name</v>
+        <v>Organization_Read_Refresh</v>
       </c>
       <c r="E141" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Organization_Write_Name,</v>
+        <v>Organization_Read_Refresh,</v>
       </c>
       <c r="F141" s="1" t="s">
         <v>147</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H141" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Organization_Write_Name, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_id"})},</v>
+        <v>{EntityRequestType.Organization_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"organizations","_id"})},</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -5767,28 +5770,28 @@
         <v>89</v>
       </c>
       <c r="B146" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C146" t="s">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="D146" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>OrganizationPreferences_Read_Refresh</v>
+        <v>OrganizationPreferences_Write_AssociatedDomain</v>
       </c>
       <c r="E146" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>OrganizationPreferences_Read_Refresh,</v>
+        <v>OrganizationPreferences_Write_AssociatedDomain,</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H146" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.OrganizationPreferences_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"organizations","_organizationId","prefs"})},</v>
+        <v>{EntityRequestType.OrganizationPreferences_Write_AssociatedDomain, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_organizationId","prefs","associatedDomain"})},</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -5799,25 +5802,25 @@
         <v>12</v>
       </c>
       <c r="C147" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D147" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>OrganizationPreferences_Write_AssociatedDomain</v>
+        <v>OrganizationPreferences_Write_ExternalMembersDisabled</v>
       </c>
       <c r="E147" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>OrganizationPreferences_Write_AssociatedDomain,</v>
+        <v>OrganizationPreferences_Write_ExternalMembersDisabled,</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G147" s="1" t="s">
         <v>171</v>
       </c>
       <c r="H147" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.OrganizationPreferences_Write_AssociatedDomain, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_organizationId","prefs","associatedDomain"})},</v>
+        <v>{EntityRequestType.OrganizationPreferences_Write_ExternalMembersDisabled, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_organizationId","prefs","externalMembersDisabled"})},</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -5828,25 +5831,25 @@
         <v>12</v>
       </c>
       <c r="C148" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D148" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>OrganizationPreferences_Write_ExternalMembersDisabled</v>
+        <v>OrganizationPreferences_Write_OrgInviteRestrict</v>
       </c>
       <c r="E148" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>OrganizationPreferences_Write_ExternalMembersDisabled,</v>
+        <v>OrganizationPreferences_Write_OrgInviteRestrict,</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G148" s="1" t="s">
         <v>171</v>
       </c>
       <c r="H148" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.OrganizationPreferences_Write_ExternalMembersDisabled, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_organizationId","prefs","externalMembersDisabled"})},</v>
+        <v>{EntityRequestType.OrganizationPreferences_Write_OrgInviteRestrict, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_organizationId","prefs","orgInviteRestrict"})},</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -5857,25 +5860,25 @@
         <v>12</v>
       </c>
       <c r="C149" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D149" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>OrganizationPreferences_Write_OrgInviteRestrict</v>
+        <v>OrganizationPreferences_Write_OrgVisibleBoardVisibility</v>
       </c>
       <c r="E149" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>OrganizationPreferences_Write_OrgInviteRestrict,</v>
+        <v>OrganizationPreferences_Write_OrgVisibleBoardVisibility,</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G149" s="1" t="s">
         <v>171</v>
       </c>
       <c r="H149" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.OrganizationPreferences_Write_OrgInviteRestrict, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_organizationId","prefs","orgInviteRestrict"})},</v>
+        <v>{EntityRequestType.OrganizationPreferences_Write_OrgVisibleBoardVisibility, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_organizationId","prefs","boardVisibilityRestrict","org"})},</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -5886,25 +5889,25 @@
         <v>12</v>
       </c>
       <c r="C150" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="D150" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>OrganizationPreferences_Write_OrgVisibleBoardVisibility</v>
+        <v>OrganizationPreferences_Write_PermissionLevel</v>
       </c>
       <c r="E150" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>OrganizationPreferences_Write_OrgVisibleBoardVisibility,</v>
+        <v>OrganizationPreferences_Write_PermissionLevel,</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G150" s="1" t="s">
         <v>171</v>
       </c>
       <c r="H150" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.OrganizationPreferences_Write_OrgVisibleBoardVisibility, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_organizationId","prefs","boardVisibilityRestrict","org"})},</v>
+        <v>{EntityRequestType.OrganizationPreferences_Write_PermissionLevel, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_organizationId","prefs","permissionLevel"})},</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -5915,25 +5918,25 @@
         <v>12</v>
       </c>
       <c r="C151" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="D151" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>OrganizationPreferences_Write_PermissionLevel</v>
+        <v>OrganizationPreferences_Write_PrivateBoardVisibility</v>
       </c>
       <c r="E151" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>OrganizationPreferences_Write_PermissionLevel,</v>
+        <v>OrganizationPreferences_Write_PrivateBoardVisibility,</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G151" s="1" t="s">
         <v>171</v>
       </c>
       <c r="H151" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.OrganizationPreferences_Write_PermissionLevel, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_organizationId","prefs","permissionLevel"})},</v>
+        <v>{EntityRequestType.OrganizationPreferences_Write_PrivateBoardVisibility, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_organizationId","prefs","boardVisibilityRestrict","private"})},</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -5944,25 +5947,25 @@
         <v>12</v>
       </c>
       <c r="C152" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D152" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>OrganizationPreferences_Write_PrivateBoardVisibility</v>
+        <v>OrganizationPreferences_Write_PublicBoardVisibility</v>
       </c>
       <c r="E152" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>OrganizationPreferences_Write_PrivateBoardVisibility,</v>
+        <v>OrganizationPreferences_Write_PublicBoardVisibility,</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G152" s="1" t="s">
         <v>171</v>
       </c>
       <c r="H152" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.OrganizationPreferences_Write_PrivateBoardVisibility, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_organizationId","prefs","boardVisibilityRestrict","private"})},</v>
+        <v>{EntityRequestType.OrganizationPreferences_Write_PublicBoardVisibility, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_organizationId","prefs","boardVisibilityRestrict","public"})},</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -5970,28 +5973,28 @@
         <v>89</v>
       </c>
       <c r="B153" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C153" t="s">
-        <v>95</v>
+        <v>4</v>
       </c>
       <c r="D153" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>OrganizationPreferences_Write_PublicBoardVisibility</v>
+        <v>OrganizationPreferences_Read_Refresh</v>
       </c>
       <c r="E153" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>OrganizationPreferences_Write_PublicBoardVisibility,</v>
+        <v>OrganizationPreferences_Read_Refresh,</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H153" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.OrganizationPreferences_Write_PublicBoardVisibility, () =&gt; new Endpoint(RestMethod.Put, new[]{"organizations","_organizationId","prefs","boardVisibilityRestrict","public"})},</v>
+        <v>{EntityRequestType.OrganizationPreferences_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"organizations","_organizationId","prefs"})},</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -6086,28 +6089,28 @@
         <v>98</v>
       </c>
       <c r="B157" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C157" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D157" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Token_Read_Refresh</v>
+        <v>Token_Write_Delete</v>
       </c>
       <c r="E157" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Token_Read_Refresh,</v>
+        <v>Token_Write_Delete,</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>186</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>168</v>
+        <v>17</v>
       </c>
       <c r="H157" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Token_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"tokens","_token"})},</v>
+        <v>{EntityRequestType.Token_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"tokens","_token"})},</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -6115,28 +6118,28 @@
         <v>98</v>
       </c>
       <c r="B158" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C158" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D158" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Token_Write_Delete</v>
+        <v>Token_Read_Refresh</v>
       </c>
       <c r="E158" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Token_Write_Delete,</v>
+        <v>Token_Read_Refresh,</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>186</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>17</v>
+        <v>168</v>
       </c>
       <c r="H158" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Token_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"tokens","_token"})},</v>
+        <v>{EntityRequestType.Token_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"tokens","_token"})},</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -6144,28 +6147,28 @@
         <v>375</v>
       </c>
       <c r="B159" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C159" t="s">
-        <v>4</v>
+        <v>377</v>
       </c>
       <c r="D159" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Webhook_Read_Refresh</v>
+        <v>Webhook_Write_Active</v>
       </c>
       <c r="E159" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Webhook_Read_Refresh,</v>
+        <v>Webhook_Write_Active,</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>376</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H159" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Webhook_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"webhooks","_id"})},</v>
+        <v>{EntityRequestType.Webhook_Write_Active, () =&gt; new Endpoint(RestMethod.Put, new[]{"webhooks","_id"})},</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -6176,15 +6179,15 @@
         <v>12</v>
       </c>
       <c r="C160" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D160" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Webhook_Write_Active</v>
+        <v>Webhook_Write_CallbackUrl</v>
       </c>
       <c r="E160" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Webhook_Write_Active,</v>
+        <v>Webhook_Write_CallbackUrl,</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>376</v>
@@ -6194,7 +6197,7 @@
       </c>
       <c r="H160" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Webhook_Write_Active, () =&gt; new Endpoint(RestMethod.Put, new[]{"webhooks","_id"})},</v>
+        <v>{EntityRequestType.Webhook_Write_CallbackUrl, () =&gt; new Endpoint(RestMethod.Put, new[]{"webhooks","_id"})},</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -6205,25 +6208,25 @@
         <v>12</v>
       </c>
       <c r="C161" t="s">
-        <v>378</v>
+        <v>17</v>
       </c>
       <c r="D161" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Webhook_Write_CallbackUrl</v>
+        <v>Webhook_Write_Delete</v>
       </c>
       <c r="E161" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Webhook_Write_CallbackUrl,</v>
+        <v>Webhook_Write_Delete,</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>376</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>171</v>
+        <v>17</v>
       </c>
       <c r="H161" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Webhook_Write_CallbackUrl, () =&gt; new Endpoint(RestMethod.Put, new[]{"webhooks","_id"})},</v>
+        <v>{EntityRequestType.Webhook_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"webhooks","_id"})},</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -6234,25 +6237,25 @@
         <v>12</v>
       </c>
       <c r="C162" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D162" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Webhook_Write_Delete</v>
+        <v>Webhook_Write_Description</v>
       </c>
       <c r="E162" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Webhook_Write_Delete,</v>
+        <v>Webhook_Write_Description,</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>376</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="H162" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Webhook_Write_Delete, () =&gt; new Endpoint(RestMethod.Delete, new[]{"webhooks","_id"})},</v>
+        <v>{EntityRequestType.Webhook_Write_Description, () =&gt; new Endpoint(RestMethod.Put, new[]{"webhooks","_id"})},</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -6263,25 +6266,25 @@
         <v>12</v>
       </c>
       <c r="C163" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D163" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Webhook_Write_Description</v>
+        <v>Webhook_Write_Entity</v>
       </c>
       <c r="E163" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Webhook_Write_Description,</v>
+        <v>Webhook_Write_Entity,</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="G163" s="1" t="s">
         <v>171</v>
       </c>
       <c r="H163" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Webhook_Write_Description, () =&gt; new Endpoint(RestMethod.Put, new[]{"webhooks","_id"})},</v>
+        <v>{EntityRequestType.Webhook_Write_Entity, () =&gt; new Endpoint(RestMethod.Put, new[]{"webhooks"})},</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
@@ -6289,28 +6292,28 @@
         <v>375</v>
       </c>
       <c r="B164" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C164" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D164" s="1" t="str">
         <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
-        <v>Webhook_Write_Entity</v>
+        <v>Webhook_Read_Refresh</v>
       </c>
       <c r="E164" s="1" t="str">
         <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
-        <v>Webhook_Write_Entity,</v>
+        <v>Webhook_Read_Refresh,</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H164" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
-        <v>{EntityRequestType.Webhook_Write_Entity, () =&gt; new Endpoint(RestMethod.Put, new[]{"webhooks"})},</v>
+        <v>{EntityRequestType.Webhook_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"webhooks","_id"})},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BUG FIX: Webhook not downloading. BUG FIX: Lists not utilizing caching for contained entities when refreshing. Added TrelloServiceConfiguration.ThrowOnTrelloError.
</commit_message>
<xml_diff>
--- a/Endpoint definitions.xlsx
+++ b/Endpoint definitions.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="387">
   <si>
     <t>Entity</t>
   </si>
@@ -1185,6 +1185,12 @@
   </si>
   <si>
     <t>"members","_id","boardStars"</t>
+  </si>
+  <si>
+    <t>CardsForMember</t>
+  </si>
+  <si>
+    <t>"board","_id","members","_memberId","cards"</t>
   </si>
 </sst>
 </file>
@@ -1257,8 +1263,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H164" totalsRowShown="0">
-  <autoFilter ref="A1:H164"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H165" totalsRowShown="0">
+  <autoFilter ref="A1:H165"/>
   <sortState ref="A2:H165">
     <sortCondition ref="A1:A165"/>
   </sortState>
@@ -1545,11 +1551,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H164"/>
+  <dimension ref="A1:H165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A113" sqref="A113:XFD113"/>
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H165" sqref="H165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6314,6 +6320,35 @@
       <c r="H164" s="1" t="str">
         <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
         <v>{EntityRequestType.Webhook_Read_Refresh, () =&gt; new Endpoint(RestMethod.Get, new[]{"webhooks","_id"})},</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>8</v>
+      </c>
+      <c r="B165" t="s">
+        <v>11</v>
+      </c>
+      <c r="C165" t="s">
+        <v>385</v>
+      </c>
+      <c r="D165" s="1" t="str">
+        <f>Table2[[#This Row],[Entity]]&amp;"_"&amp;Table2[[#This Row],[R/W]]&amp;"_"&amp;Table2[[#This Row],[Requested Action]]</f>
+        <v>Board_Read_CardsForMember</v>
+      </c>
+      <c r="E165" s="1" t="str">
+        <f>Table2[[#This Row],[Enum Value]]&amp;","</f>
+        <v>Board_Read_CardsForMember,</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H165" s="1" t="str">
+        <f>"{EntityRequestType."&amp;Table2[[#This Row],[Enum Value]]&amp;", () =&gt; new Endpoint(RestMethod."&amp;Table2[[#This Row],[Method]]&amp;", new[]{"&amp;Table2[[#This Row],[Endpoint]]&amp;"})},"</f>
+        <v>{EntityRequestType.Board_Read_CardsForMember, () =&gt; new Endpoint(RestMethod.Get, new[]{"board","_id","members","_memberId","cards"})},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>